<commit_message>
add metrics sheet to test plan
</commit_message>
<xml_diff>
--- a/test-plan.xlsx
+++ b/test-plan.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED1D9E9-67A6-E249-8420-0A06F5145B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="IntegrationTests" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="IntegrationTests" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Metrics" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="437">
   <si>
     <t>S.NO.</t>
   </si>
@@ -845,6 +842,24 @@
     <t xml:space="preserve">Data Explorer </t>
   </si>
   <si>
+    <t xml:space="preserve">  ☐ Faceted search - Numeric fields in faceted search are displayed as a slider @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Text fields in faceted search are displayed as checkboxes @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Filters can be organized in multiple tabs @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Display names can be set for the filters @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Data shown in charts corresponds to filters set @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Nested data - Nested fields can be shown @manual</t>
+  </si>
+  <si>
     <t>SUITE 35</t>
   </si>
   <si>
@@ -1299,36 +1314,39 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>SUITES</t>
+  </si>
+  <si>
+    <t>TESTS</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1694,24 +1712,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G376"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A376" sqref="A376"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="195" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-  </cols>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G382"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1734,7 +1739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1742,7 +1747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1753,7 +1758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1764,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1775,7 +1780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1786,7 +1791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1805,7 +1810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1816,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1827,7 +1832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1835,7 +1840,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1846,7 +1851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1857,7 +1862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1865,7 +1870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>10</v>
       </c>
@@ -1876,7 +1881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>11</v>
       </c>
@@ -1887,7 +1892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>12</v>
       </c>
@@ -1898,7 +1903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1906,7 +1911,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>13</v>
       </c>
@@ -1923,7 +1928,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -1940,7 +1945,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>15</v>
       </c>
@@ -1957,7 +1962,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>16</v>
       </c>
@@ -1974,7 +1979,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>17</v>
       </c>
@@ -1991,7 +1996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>18</v>
       </c>
@@ -2008,7 +2013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>19</v>
       </c>
@@ -2025,7 +2030,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>20</v>
       </c>
@@ -2042,7 +2047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>21</v>
       </c>
@@ -2059,7 +2064,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>22</v>
       </c>
@@ -2076,7 +2081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>23</v>
       </c>
@@ -2093,7 +2098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>24</v>
       </c>
@@ -2110,7 +2115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>25</v>
       </c>
@@ -2127,7 +2132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>26</v>
       </c>
@@ -2144,7 +2149,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>27</v>
       </c>
@@ -2161,7 +2166,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>28</v>
       </c>
@@ -2178,7 +2183,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>29</v>
       </c>
@@ -2197,7 +2202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>30</v>
       </c>
@@ -2208,7 +2213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>31</v>
       </c>
@@ -2219,7 +2224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>32</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>33</v>
       </c>
@@ -2241,7 +2246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>34</v>
       </c>
@@ -2252,7 +2257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>35</v>
       </c>
@@ -2263,7 +2268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>36</v>
       </c>
@@ -2274,7 +2279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>37</v>
       </c>
@@ -2285,7 +2290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>38</v>
       </c>
@@ -2296,7 +2301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>39</v>
       </c>
@@ -2307,7 +2312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>40</v>
       </c>
@@ -2318,7 +2323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>41</v>
       </c>
@@ -2329,7 +2334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>42</v>
       </c>
@@ -2340,7 +2345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>43</v>
       </c>
@@ -2351,7 +2356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>44</v>
       </c>
@@ -2362,7 +2367,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>45</v>
       </c>
@@ -2373,7 +2378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>46</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>47</v>
       </c>
@@ -2395,7 +2400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>48</v>
       </c>
@@ -2406,7 +2411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>49</v>
       </c>
@@ -2417,7 +2422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>71</v>
       </c>
@@ -2425,7 +2430,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>50</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>51</v>
       </c>
@@ -2459,7 +2464,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>52</v>
       </c>
@@ -2476,7 +2481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>53</v>
       </c>
@@ -2493,7 +2498,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>54</v>
       </c>
@@ -2510,7 +2515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>55</v>
       </c>
@@ -2527,7 +2532,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>56</v>
       </c>
@@ -2544,7 +2549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>57</v>
       </c>
@@ -2561,7 +2566,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>81</v>
       </c>
@@ -2569,7 +2574,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>58</v>
       </c>
@@ -2586,7 +2591,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>59</v>
       </c>
@@ -2603,7 +2608,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>60</v>
       </c>
@@ -2620,7 +2625,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>61</v>
       </c>
@@ -2637,7 +2642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>87</v>
       </c>
@@ -2645,7 +2650,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>62</v>
       </c>
@@ -2656,7 +2661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>63</v>
       </c>
@@ -2667,7 +2672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>64</v>
       </c>
@@ -2678,7 +2683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>65</v>
       </c>
@@ -2689,7 +2694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>66</v>
       </c>
@@ -2700,7 +2705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>67</v>
       </c>
@@ -2711,7 +2716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>68</v>
       </c>
@@ -2722,7 +2727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>69</v>
       </c>
@@ -2733,7 +2738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -2741,7 +2746,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>70</v>
       </c>
@@ -2752,7 +2757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>71</v>
       </c>
@@ -2763,7 +2768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>72</v>
       </c>
@@ -2774,7 +2779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>101</v>
       </c>
@@ -2782,7 +2787,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>73</v>
       </c>
@@ -2799,7 +2804,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>74</v>
       </c>
@@ -2816,7 +2821,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>75</v>
       </c>
@@ -2833,7 +2838,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>76</v>
       </c>
@@ -2850,7 +2855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>77</v>
       </c>
@@ -2867,7 +2872,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>108</v>
       </c>
@@ -2875,7 +2880,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>78</v>
       </c>
@@ -2892,7 +2897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>79</v>
       </c>
@@ -2909,7 +2914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>112</v>
       </c>
@@ -2917,7 +2922,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>80</v>
       </c>
@@ -2934,7 +2939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>115</v>
       </c>
@@ -2942,7 +2947,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>81</v>
       </c>
@@ -2959,7 +2964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>82</v>
       </c>
@@ -2976,7 +2981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>83</v>
       </c>
@@ -2993,7 +2998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>84</v>
       </c>
@@ -3010,7 +3015,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>85</v>
       </c>
@@ -3027,7 +3032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>86</v>
       </c>
@@ -3044,7 +3049,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>87</v>
       </c>
@@ -3061,7 +3066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>124</v>
       </c>
@@ -3069,7 +3074,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>88</v>
       </c>
@@ -3086,7 +3091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>89</v>
       </c>
@@ -3103,7 +3108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>90</v>
       </c>
@@ -3120,7 +3125,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>91</v>
       </c>
@@ -3137,7 +3142,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>92</v>
       </c>
@@ -3154,7 +3159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>93</v>
       </c>
@@ -3171,7 +3176,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>94</v>
       </c>
@@ -3188,7 +3193,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>95</v>
       </c>
@@ -3205,7 +3210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>96</v>
       </c>
@@ -3222,7 +3227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="113" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>97</v>
       </c>
@@ -3239,7 +3244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>98</v>
       </c>
@@ -3256,7 +3261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>99</v>
       </c>
@@ -3273,7 +3278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>100</v>
       </c>
@@ -3290,7 +3295,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>101</v>
       </c>
@@ -3307,7 +3312,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>102</v>
       </c>
@@ -3324,7 +3329,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>141</v>
       </c>
@@ -3332,7 +3337,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="120" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>103</v>
       </c>
@@ -3349,7 +3354,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>104</v>
       </c>
@@ -3366,7 +3371,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>105</v>
       </c>
@@ -3383,7 +3388,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>106</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>107</v>
       </c>
@@ -3417,7 +3422,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>108</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="126" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>109</v>
       </c>
@@ -3451,7 +3456,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="127" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>150</v>
       </c>
@@ -3459,7 +3464,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="128" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>110</v>
       </c>
@@ -3476,7 +3481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="129" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>111</v>
       </c>
@@ -3493,7 +3498,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>112</v>
       </c>
@@ -3510,7 +3515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>113</v>
       </c>
@@ -3527,7 +3532,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="132" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>114</v>
       </c>
@@ -3544,7 +3549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>157</v>
       </c>
@@ -3552,7 +3557,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>115</v>
       </c>
@@ -3563,7 +3568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>116</v>
       </c>
@@ -3574,7 +3579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>117</v>
       </c>
@@ -3585,7 +3590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>118</v>
       </c>
@@ -3596,7 +3601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>119</v>
       </c>
@@ -3607,7 +3612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>120</v>
       </c>
@@ -3618,7 +3623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>121</v>
       </c>
@@ -3629,7 +3634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>122</v>
       </c>
@@ -3640,7 +3645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>123</v>
       </c>
@@ -3651,7 +3656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>124</v>
       </c>
@@ -3662,7 +3667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>125</v>
       </c>
@@ -3673,7 +3678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>170</v>
       </c>
@@ -3681,7 +3686,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="146" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>126</v>
       </c>
@@ -3692,7 +3697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>127</v>
       </c>
@@ -3703,7 +3708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>128</v>
       </c>
@@ -3714,7 +3719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>129</v>
       </c>
@@ -3725,7 +3730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>130</v>
       </c>
@@ -3736,7 +3741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>131</v>
       </c>
@@ -3747,7 +3752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>132</v>
       </c>
@@ -3758,7 +3763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>179</v>
       </c>
@@ -3766,7 +3771,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="154" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>133</v>
       </c>
@@ -3777,7 +3782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>134</v>
       </c>
@@ -3788,7 +3793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>183</v>
       </c>
@@ -3796,7 +3801,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="157" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>135</v>
       </c>
@@ -3813,7 +3818,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="158" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>186</v>
       </c>
@@ -3821,7 +3826,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="159" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>136</v>
       </c>
@@ -3832,7 +3837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>137</v>
       </c>
@@ -3843,7 +3848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>138</v>
       </c>
@@ -3854,7 +3859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>139</v>
       </c>
@@ -3865,7 +3870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>140</v>
       </c>
@@ -3876,7 +3881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>141</v>
       </c>
@@ -3887,7 +3892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>142</v>
       </c>
@@ -3898,7 +3903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>143</v>
       </c>
@@ -3909,7 +3914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>144</v>
       </c>
@@ -3920,7 +3925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>193</v>
       </c>
@@ -3928,7 +3933,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="169" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>145</v>
       </c>
@@ -3945,7 +3950,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="170" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>146</v>
       </c>
@@ -3962,7 +3967,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="171" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>147</v>
       </c>
@@ -3979,7 +3984,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="172" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>198</v>
       </c>
@@ -3987,7 +3992,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="173" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>148</v>
       </c>
@@ -4004,7 +4009,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="174" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>149</v>
       </c>
@@ -4021,7 +4026,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="175" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>150</v>
       </c>
@@ -4038,7 +4043,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="176" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>151</v>
       </c>
@@ -4055,7 +4060,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="177" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>152</v>
       </c>
@@ -4072,7 +4077,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="178" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>205</v>
       </c>
@@ -4080,7 +4085,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="179" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>153</v>
       </c>
@@ -4097,7 +4102,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="180" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>154</v>
       </c>
@@ -4114,7 +4119,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="181" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>155</v>
       </c>
@@ -4131,7 +4136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>156</v>
       </c>
@@ -4148,7 +4153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="183" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>157</v>
       </c>
@@ -4165,7 +4170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>212</v>
       </c>
@@ -4173,7 +4178,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="185" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>158</v>
       </c>
@@ -4190,7 +4195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>159</v>
       </c>
@@ -4207,7 +4212,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="187" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>160</v>
       </c>
@@ -4224,7 +4229,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>161</v>
       </c>
@@ -4241,7 +4246,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="189" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>162</v>
       </c>
@@ -4258,7 +4263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="190" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>163</v>
       </c>
@@ -4275,7 +4280,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="191" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>164</v>
       </c>
@@ -4292,7 +4297,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="192" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>165</v>
       </c>
@@ -4309,7 +4314,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="193" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>166</v>
       </c>
@@ -4326,7 +4331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="194" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>167</v>
       </c>
@@ -4343,7 +4348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>168</v>
       </c>
@@ -4360,7 +4365,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="196" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>169</v>
       </c>
@@ -4377,7 +4382,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="197" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>170</v>
       </c>
@@ -4394,7 +4399,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="198" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>171</v>
       </c>
@@ -4411,7 +4416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="199" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>172</v>
       </c>
@@ -4428,7 +4433,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="200" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>173</v>
       </c>
@@ -4445,7 +4450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="201" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>174</v>
       </c>
@@ -4462,7 +4467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="202" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>175</v>
       </c>
@@ -4479,7 +4484,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="203" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>232</v>
       </c>
@@ -4487,7 +4492,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="204" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>176</v>
       </c>
@@ -4504,7 +4509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="205" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>177</v>
       </c>
@@ -4521,7 +4526,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="206" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>178</v>
       </c>
@@ -4538,7 +4543,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="207" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>179</v>
       </c>
@@ -4555,7 +4560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="208" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>180</v>
       </c>
@@ -4572,7 +4577,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="209" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>181</v>
       </c>
@@ -4589,7 +4594,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="210" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>182</v>
       </c>
@@ -4606,7 +4611,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="211" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>241</v>
       </c>
@@ -4614,7 +4619,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="212" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>183</v>
       </c>
@@ -4625,7 +4630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>184</v>
       </c>
@@ -4636,7 +4641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>185</v>
       </c>
@@ -4647,7 +4652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>186</v>
       </c>
@@ -4658,7 +4663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>187</v>
       </c>
@@ -4669,7 +4674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>248</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="218" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>188</v>
       </c>
@@ -4688,7 +4693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>189</v>
       </c>
@@ -4699,7 +4704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>190</v>
       </c>
@@ -4710,7 +4715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>191</v>
       </c>
@@ -4721,7 +4726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>192</v>
       </c>
@@ -4732,7 +4737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>254</v>
       </c>
@@ -4740,7 +4745,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="224" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>193</v>
       </c>
@@ -4751,7 +4756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>194</v>
       </c>
@@ -4762,7 +4767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>195</v>
       </c>
@@ -4773,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>259</v>
       </c>
@@ -4781,7 +4786,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="228" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>196</v>
       </c>
@@ -4798,7 +4803,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="229" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>197</v>
       </c>
@@ -4815,7 +4820,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="230" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3">
         <v>198</v>
       </c>
@@ -4832,7 +4837,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="231" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>264</v>
       </c>
@@ -4840,7 +4845,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="232" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>199</v>
       </c>
@@ -4857,7 +4862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="233" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>267</v>
       </c>
@@ -4865,7 +4870,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="234" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>200</v>
       </c>
@@ -4876,7 +4881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>201</v>
       </c>
@@ -4887,7 +4892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>202</v>
       </c>
@@ -4898,7 +4903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>203</v>
       </c>
@@ -4909,7 +4914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>204</v>
       </c>
@@ -4920,7 +4925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="239" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>274</v>
       </c>
@@ -4928,484 +4933,484 @@
         <v>275</v>
       </c>
     </row>
-    <row r="240" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A240" s="2" t="s">
+    <row r="240" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="3">
+        <v>205</v>
+      </c>
+      <c r="B240" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="C240" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="3">
+        <v>206</v>
+      </c>
+      <c r="B241" s="3" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="241" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A241" s="3">
-        <v>205</v>
-      </c>
-      <c r="B241" s="3" t="s">
+      <c r="C241" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="3">
+        <v>207</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C241" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E241" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F241" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A242" s="3">
-        <v>206</v>
-      </c>
-      <c r="B242" s="3" t="s">
+      <c r="C242" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="3">
+        <v>208</v>
+      </c>
+      <c r="B243" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C242" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E242" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F242" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A243" s="3">
-        <v>207</v>
-      </c>
-      <c r="B243" s="3" t="s">
+      <c r="C243" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="3">
+        <v>209</v>
+      </c>
+      <c r="B244" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C243" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
+      <c r="C244" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="3">
+        <v>210</v>
+      </c>
+      <c r="B245" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="C245" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A245" s="3">
-        <v>208</v>
-      </c>
-      <c r="B245" s="3" t="s">
+      <c r="B246" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C245" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A246" s="3">
-        <v>209</v>
-      </c>
-      <c r="B246" s="3" t="s">
+    </row>
+    <row r="247" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="3">
+        <v>211</v>
+      </c>
+      <c r="B247" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C246" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A247" s="3">
-        <v>210</v>
-      </c>
-      <c r="B247" s="3" t="s">
+      <c r="C247" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F247" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="3">
+        <v>212</v>
+      </c>
+      <c r="B248" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C247" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A248" s="3">
-        <v>211</v>
-      </c>
-      <c r="B248" s="3" t="s">
+      <c r="C248" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="3">
+        <v>213</v>
+      </c>
+      <c r="B249" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C248" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
+      <c r="C249" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B249" s="2" t="s">
+      <c r="B250" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="250" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A250" s="3">
-        <v>212</v>
-      </c>
-      <c r="B250" s="3" t="s">
+    <row r="251" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="3">
+        <v>214</v>
+      </c>
+      <c r="B251" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C250" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A251" s="3">
-        <v>213</v>
-      </c>
-      <c r="B251" s="3" t="s">
+      <c r="C251" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="3">
+        <v>215</v>
+      </c>
+      <c r="B252" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A252" s="3">
-        <v>214</v>
-      </c>
-      <c r="B252" s="3" t="s">
+      <c r="C252" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="3">
+        <v>216</v>
+      </c>
+      <c r="B253" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C252" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A253" s="3">
-        <v>215</v>
-      </c>
-      <c r="B253" s="3" t="s">
+      <c r="C253" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="3">
+        <v>217</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="C253" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A254" s="3">
-        <v>216</v>
-      </c>
-      <c r="B254" s="3" t="s">
+      <c r="C254" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C254" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A255" s="3">
-        <v>217</v>
-      </c>
-      <c r="B255" s="3" t="s">
+      <c r="B255" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C255" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A256" s="2" t="s">
+    </row>
+    <row r="256" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="3">
+        <v>218</v>
+      </c>
+      <c r="B256" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B256" s="2" t="s">
+      <c r="C256" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="3">
+        <v>219</v>
+      </c>
+      <c r="B257" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A257" s="3">
-        <v>218</v>
-      </c>
-      <c r="B257" s="3" t="s">
+      <c r="C257" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="3">
+        <v>220</v>
+      </c>
+      <c r="B258" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C257" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A258" s="3">
-        <v>219</v>
-      </c>
-      <c r="B258" s="3" t="s">
+      <c r="C258" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="3">
+        <v>221</v>
+      </c>
+      <c r="B259" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="C258" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A259" s="3">
-        <v>220</v>
-      </c>
-      <c r="B259" s="3" t="s">
+      <c r="C259" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="3">
+        <v>222</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C259" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A260" s="3">
-        <v>221</v>
-      </c>
-      <c r="B260" s="3" t="s">
+      <c r="C260" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="3">
+        <v>223</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C260" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A261" s="3">
-        <v>222</v>
-      </c>
-      <c r="B261" s="3" t="s">
+      <c r="C261" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C261" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
+      <c r="B262" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B262" s="2" t="s">
+    </row>
+    <row r="263" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="3">
+        <v>224</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A263" s="3">
-        <v>223</v>
-      </c>
-      <c r="B263" s="3" t="s">
+      <c r="C263" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="3">
+        <v>225</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="C263" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E263" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F263" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A264" s="3">
-        <v>224</v>
-      </c>
-      <c r="B264" s="3" t="s">
+      <c r="C264" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="3">
+        <v>226</v>
+      </c>
+      <c r="B265" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="C264" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E264" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F264" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A265" s="2" t="s">
+      <c r="C265" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="3">
+        <v>227</v>
+      </c>
+      <c r="B266" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B265" s="2" t="s">
+      <c r="C266" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="3">
+        <v>228</v>
+      </c>
+      <c r="B267" s="3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A266" s="3">
-        <v>225</v>
-      </c>
-      <c r="B266" s="3" t="s">
+      <c r="C267" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C266" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E266" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F266" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A267" s="3">
-        <v>226</v>
-      </c>
-      <c r="B267" s="3" t="s">
+      <c r="B268" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C267" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E267" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F267" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A268" s="2" t="s">
+    </row>
+    <row r="269" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="3">
+        <v>229</v>
+      </c>
+      <c r="B269" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B268" s="2" t="s">
+      <c r="C269" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E269" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F269" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="3">
+        <v>230</v>
+      </c>
+      <c r="B270" s="3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="269" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A269" s="3">
-        <v>227</v>
-      </c>
-      <c r="B269" s="3" t="s">
+      <c r="C270" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E270" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F270" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C269" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E269" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F269" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A270" s="2" t="s">
+      <c r="B271" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B270" s="2" t="s">
+    </row>
+    <row r="272" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="3">
+        <v>231</v>
+      </c>
+      <c r="B272" s="3" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="271" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A271" s="3">
-        <v>228</v>
-      </c>
-      <c r="B271" s="3" t="s">
+      <c r="C272" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E272" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F272" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="3">
+        <v>232</v>
+      </c>
+      <c r="B273" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C271" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A272" s="3">
-        <v>229</v>
-      </c>
-      <c r="B272" s="3" t="s">
+      <c r="C273" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E273" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F273" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C272" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A273" s="3">
-        <v>230</v>
-      </c>
-      <c r="B273" s="3" t="s">
+      <c r="B274" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C273" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A274" s="3">
-        <v>231</v>
-      </c>
-      <c r="B274" s="3" t="s">
+    </row>
+    <row r="275" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="3">
+        <v>233</v>
+      </c>
+      <c r="B275" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="C274" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A275" s="2" t="s">
+      <c r="C275" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E275" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F275" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B275" s="2" t="s">
+      <c r="B276" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="276" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A276" s="3">
-        <v>232</v>
-      </c>
-      <c r="B276" s="3" t="s">
+    <row r="277" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="3">
+        <v>234</v>
+      </c>
+      <c r="B277" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C276" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A277" s="3">
-        <v>233</v>
-      </c>
-      <c r="B277" s="3" t="s">
+      <c r="C277" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="3">
+        <v>235</v>
+      </c>
+      <c r="B278" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="C277" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A278" s="3">
-        <v>234</v>
-      </c>
-      <c r="B278" s="3" t="s">
+      <c r="C278" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="3">
+        <v>236</v>
+      </c>
+      <c r="B279" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C278" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A279" s="3">
-        <v>235</v>
-      </c>
-      <c r="B279" s="3" t="s">
+      <c r="C279" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="3">
+        <v>237</v>
+      </c>
+      <c r="B280" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="C279" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A280" s="3">
-        <v>236</v>
-      </c>
-      <c r="B280" s="3" t="s">
+      <c r="C280" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C280" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A281" s="3">
-        <v>237</v>
-      </c>
-      <c r="B281" s="3" t="s">
+      <c r="B281" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C281" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="282" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" s="3">
         <v>238</v>
       </c>
@@ -5416,7 +5421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A283" s="3">
         <v>239</v>
       </c>
@@ -5427,7 +5432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" s="3">
         <v>240</v>
       </c>
@@ -5438,7 +5443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" s="3">
         <v>241</v>
       </c>
@@ -5449,7 +5454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" s="3">
         <v>242</v>
       </c>
@@ -5460,7 +5465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A287" s="3">
         <v>243</v>
       </c>
@@ -5471,7 +5476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="288" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="3">
         <v>244</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="289" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" s="3">
         <v>245</v>
       </c>
@@ -5493,152 +5498,155 @@
         <v>10</v>
       </c>
     </row>
-    <row r="290" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A290" s="2" t="s">
+    <row r="290" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="3">
+        <v>246</v>
+      </c>
+      <c r="B290" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="B290" s="2" t="s">
+      <c r="C290" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="3">
+        <v>247</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A291" s="3">
-        <v>246</v>
-      </c>
-      <c r="B291" s="3" t="s">
+      <c r="C291" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="3">
+        <v>248</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C291" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A292" s="3">
-        <v>247</v>
-      </c>
-      <c r="B292" s="3" t="s">
+      <c r="C292" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="3">
+        <v>249</v>
+      </c>
+      <c r="B293" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="C292" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A293" s="3">
-        <v>248</v>
-      </c>
-      <c r="B293" s="3" t="s">
+      <c r="C293" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="3">
+        <v>250</v>
+      </c>
+      <c r="B294" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C293" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A294" s="2" t="s">
+      <c r="C294" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="3">
+        <v>251</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="B294" s="2" t="s">
+      <c r="C295" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A295" s="3">
-        <v>249</v>
-      </c>
-      <c r="B295" s="3" t="s">
+      <c r="B296" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C295" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A296" s="3">
-        <v>250</v>
-      </c>
-      <c r="B296" s="3" t="s">
+    </row>
+    <row r="297" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="3">
+        <v>252</v>
+      </c>
+      <c r="B297" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="C296" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A297" s="3">
-        <v>251</v>
-      </c>
-      <c r="B297" s="3" t="s">
+      <c r="C297" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="3">
+        <v>253</v>
+      </c>
+      <c r="B298" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="C297" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A298" s="2" t="s">
+      <c r="C298" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="3">
+        <v>254</v>
+      </c>
+      <c r="B299" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="B298" s="2" t="s">
+      <c r="C299" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A299" s="3">
-        <v>252</v>
-      </c>
-      <c r="B299" s="3" t="s">
+      <c r="B300" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="C299" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A300" s="3">
-        <v>253</v>
-      </c>
-      <c r="B300" s="3" t="s">
+    </row>
+    <row r="301" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="3">
+        <v>255</v>
+      </c>
+      <c r="B301" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="C300" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A301" s="3">
-        <v>254</v>
-      </c>
-      <c r="B301" s="3" t="s">
+      <c r="C301" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="3">
+        <v>256</v>
+      </c>
+      <c r="B302" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="C301" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A302" s="3">
-        <v>255</v>
-      </c>
-      <c r="B302" s="3" t="s">
+      <c r="C302" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="3">
+        <v>257</v>
+      </c>
+      <c r="B303" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="C302" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A303" s="3">
-        <v>256</v>
-      </c>
-      <c r="B303" s="3" t="s">
-        <v>349</v>
-      </c>
       <c r="C303" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>351</v>
       </c>
@@ -5646,9 +5654,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="305" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B305" s="3" t="s">
         <v>353</v>
@@ -5657,9 +5665,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A306" s="3">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B306" s="3" t="s">
         <v>354</v>
@@ -5668,9 +5676,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A307" s="3">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B307" s="3" t="s">
         <v>355</v>
@@ -5679,9 +5687,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A308" s="3">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B308" s="3" t="s">
         <v>356</v>
@@ -5690,29 +5698,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="309" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A309" s="3">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B309" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C309" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A310" s="3">
-        <v>262</v>
-      </c>
-      <c r="B310" s="3" t="s">
+      <c r="B310" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C310" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="311" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" s="3">
         <v>263</v>
       </c>
@@ -5723,7 +5728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A312" s="3">
         <v>264</v>
       </c>
@@ -5734,83 +5739,86 @@
         <v>10</v>
       </c>
     </row>
-    <row r="313" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A313" s="3">
         <v>265</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="314" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" s="3">
         <v>266</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="315" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A315" s="3">
         <v>267</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A316" s="3">
         <v>268</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="317" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3">
         <v>269</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="318" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A318" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B318" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A318" s="3">
+        <v>270</v>
+      </c>
+      <c r="B318" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C318" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" s="3">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="320" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" s="3">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B320" s="3" t="s">
         <v>366</v>
@@ -5819,9 +5827,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="321" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" s="3">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B321" s="3" t="s">
         <v>367</v>
@@ -5830,9 +5838,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="322" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="3">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B322" s="3" t="s">
         <v>368</v>
@@ -5841,300 +5849,261 @@
         <v>10</v>
       </c>
     </row>
-    <row r="323" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B323" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C323" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C323" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A324" s="2" t="s">
+      <c r="B324" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B324" s="2" t="s">
+    </row>
+    <row r="325" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A325" s="3">
+        <v>276</v>
+      </c>
+      <c r="B325" s="3" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A325" s="3">
-        <v>275</v>
-      </c>
-      <c r="B325" s="3" t="s">
+      <c r="C325" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A326" s="3">
+        <v>277</v>
+      </c>
+      <c r="B326" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C326" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A327" s="3">
+        <v>278</v>
+      </c>
+      <c r="B327" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C327" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A328" s="3">
+        <v>279</v>
+      </c>
+      <c r="B328" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C328" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A329" s="3">
+        <v>280</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C329" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A330" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A331" s="3">
+        <v>281</v>
+      </c>
+      <c r="B331" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C325" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A326" s="3">
-        <v>276</v>
-      </c>
-      <c r="B326" s="3" t="s">
+      <c r="C331" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A332" s="3">
+        <v>282</v>
+      </c>
+      <c r="B332" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C326" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A327" s="3">
-        <v>277</v>
-      </c>
-      <c r="B327" s="3" t="s">
+      <c r="C332" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="3">
+        <v>283</v>
+      </c>
+      <c r="B333" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C327" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A328" s="3">
-        <v>278</v>
-      </c>
-      <c r="B328" s="3" t="s">
+      <c r="C333" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="3">
+        <v>284</v>
+      </c>
+      <c r="B334" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C328" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A329" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="B329" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A330" s="3">
-        <v>279</v>
-      </c>
-      <c r="B330" s="3" t="s">
+      <c r="C334" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="3">
+        <v>285</v>
+      </c>
+      <c r="B336" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C330" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="331" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A331" s="3">
-        <v>280</v>
-      </c>
-      <c r="B331" s="3" t="s">
+      <c r="C336" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="3">
+        <v>286</v>
+      </c>
+      <c r="B337" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C331" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="332" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A332" s="3">
-        <v>281</v>
-      </c>
-      <c r="B332" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="C332" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="333" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A333" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="B333" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="334" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A334" s="3">
-        <v>282</v>
-      </c>
-      <c r="B334" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="C334" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="335" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A335" s="3">
-        <v>283</v>
-      </c>
-      <c r="B335" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="C335" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A336" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="B336" s="2" t="s">
+      <c r="C337" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="3">
+        <v>287</v>
+      </c>
+      <c r="B338" s="3" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="337" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A337" s="2" t="s">
+      <c r="C338" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B337" s="2" t="s">
+      <c r="B339" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="338" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A338" s="3">
-        <v>284</v>
-      </c>
-      <c r="B338" s="3" t="s">
+    <row r="340" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="3">
+        <v>288</v>
+      </c>
+      <c r="B340" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="C338" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E338" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F338" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="339" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A339" s="2" t="s">
+      <c r="C340" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="3">
+        <v>289</v>
+      </c>
+      <c r="B341" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="B339" s="2" t="s">
+      <c r="C341" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="2" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="340" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A340" s="2" t="s">
+      <c r="B342" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B340" s="2" t="s">
+    </row>
+    <row r="343" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="341" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A341" s="2" t="s">
+      <c r="B343" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B341" s="2" t="s">
+    </row>
+    <row r="344" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="3">
+        <v>290</v>
+      </c>
+      <c r="B344" s="3" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="342" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A342" s="3">
-        <v>285</v>
-      </c>
-      <c r="B342" s="3" t="s">
+      <c r="C344" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E344" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F344" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C342" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E342" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F342" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="343" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A343" s="3">
-        <v>286</v>
-      </c>
-      <c r="B343" s="3" t="s">
+      <c r="B345" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="C343" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E343" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F343" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="344" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A344" s="3">
-        <v>287</v>
-      </c>
-      <c r="B344" s="3" t="s">
+    </row>
+    <row r="346" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="C344" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E344" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F344" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="345" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A345" s="3">
-        <v>288</v>
-      </c>
-      <c r="B345" s="3" t="s">
+      <c r="B346" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="C345" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E345" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F345" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="346" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A346" s="3">
-        <v>289</v>
-      </c>
-      <c r="B346" s="3" t="s">
+    </row>
+    <row r="347" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C346" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E346" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F346" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="347" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A347" s="3">
-        <v>290</v>
-      </c>
-      <c r="B347" s="3" t="s">
+      <c r="B347" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="C347" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E347" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F347" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="348" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="348" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3">
         <v>291</v>
       </c>
@@ -6151,7 +6120,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="349" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A349" s="3">
         <v>292</v>
       </c>
@@ -6168,7 +6137,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="350" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3">
         <v>293</v>
       </c>
@@ -6185,7 +6154,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="351" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3">
         <v>294</v>
       </c>
@@ -6202,7 +6171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="352" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3">
         <v>295</v>
       </c>
@@ -6219,7 +6188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="353" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A353" s="3">
         <v>296</v>
       </c>
@@ -6236,7 +6205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="354" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A354" s="3">
         <v>297</v>
       </c>
@@ -6253,7 +6222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="355" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A355" s="3">
         <v>298</v>
       </c>
@@ -6270,140 +6239,176 @@
         <v>33</v>
       </c>
     </row>
-    <row r="356" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A356" s="2" t="s">
+    <row r="356" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="3">
+        <v>299</v>
+      </c>
+      <c r="B356" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="B356" s="2" t="s">
+      <c r="C356" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E356" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F356" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A357" s="3">
+        <v>300</v>
+      </c>
+      <c r="B357" s="3" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="357" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A357" s="3">
-        <v>299</v>
-      </c>
-      <c r="B357" s="3" t="s">
+      <c r="C357" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E357" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F357" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="3">
+        <v>301</v>
+      </c>
+      <c r="B358" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="C357" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E357" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F357" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="358" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A358" s="3">
-        <v>300</v>
-      </c>
-      <c r="B358" s="3" t="s">
+      <c r="C358" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E358" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F358" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A359" s="3">
+        <v>302</v>
+      </c>
+      <c r="B359" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C358" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E358" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F358" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="359" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A359" s="3">
-        <v>301</v>
-      </c>
-      <c r="B359" s="3" t="s">
+      <c r="C359" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E359" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F359" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A360" s="3">
+        <v>303</v>
+      </c>
+      <c r="B360" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="C359" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E359" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F359" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="360" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A360" s="2" t="s">
+      <c r="C360" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E360" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F360" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="3">
+        <v>304</v>
+      </c>
+      <c r="B361" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="B360" s="2" t="s">
+      <c r="C361" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E361" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F361" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="2" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="361" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A361" s="3">
-        <v>302</v>
-      </c>
-      <c r="B361" s="3" t="s">
+      <c r="B362" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="C361" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A362" s="3">
-        <v>303</v>
-      </c>
-      <c r="B362" s="3" t="s">
+    </row>
+    <row r="363" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="3">
+        <v>305</v>
+      </c>
+      <c r="B363" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="C362" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="363" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A363" s="3">
-        <v>304</v>
-      </c>
-      <c r="B363" s="3" t="s">
+      <c r="C363" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E363" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F363" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="3">
+        <v>306</v>
+      </c>
+      <c r="B364" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="C363" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="364" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A364" s="3">
-        <v>305</v>
-      </c>
-      <c r="B364" s="3" t="s">
+      <c r="C364" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E364" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F364" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A365" s="3">
+        <v>307</v>
+      </c>
+      <c r="B365" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="C364" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="365" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A365" s="3">
-        <v>306</v>
-      </c>
-      <c r="B365" s="3" t="s">
+      <c r="C365" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E365" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F365" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C365" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="366" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A366" s="3">
-        <v>307</v>
-      </c>
-      <c r="B366" s="3" t="s">
+      <c r="B366" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C366" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="367" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="367" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A367" s="3">
         <v>308</v>
       </c>
@@ -6414,7 +6419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="368" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A368" s="3">
         <v>309</v>
       </c>
@@ -6425,7 +6430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="369" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A369" s="3">
         <v>310</v>
       </c>
@@ -6436,7 +6441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="370" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A370" s="3">
         <v>311</v>
       </c>
@@ -6447,7 +6452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="371" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A371" s="3">
         <v>312</v>
       </c>
@@ -6458,7 +6463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="372" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A372" s="3">
         <v>313</v>
       </c>
@@ -6469,7 +6474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="373" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A373" s="3">
         <v>314</v>
       </c>
@@ -6480,7 +6485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="374" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A374" s="3">
         <v>315</v>
       </c>
@@ -6491,7 +6496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="375" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3">
         <v>316</v>
       </c>
@@ -6502,16 +6507,125 @@
         <v>10</v>
       </c>
     </row>
-    <row r="376" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A376" s="2" t="s">
+    <row r="376" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A376" s="3">
+        <v>317</v>
+      </c>
+      <c r="B376" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="B376" s="2" t="s">
+      <c r="C376" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A377" s="3">
+        <v>318</v>
+      </c>
+      <c r="B377" s="3" t="s">
         <v>427</v>
+      </c>
+      <c r="C377" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A378" s="3">
+        <v>319</v>
+      </c>
+      <c r="B378" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C378" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A379" s="3">
+        <v>320</v>
+      </c>
+      <c r="B379" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C379" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A380" s="3">
+        <v>321</v>
+      </c>
+      <c r="B380" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C380" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A381" s="3">
+        <v>322</v>
+      </c>
+      <c r="B381" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C381" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add metrics sheet to test plan (#359)
</commit_message>
<xml_diff>
--- a/test-plan.xlsx
+++ b/test-plan.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED1D9E9-67A6-E249-8420-0A06F5145B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="IntegrationTests" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="IntegrationTests" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Metrics" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="437">
   <si>
     <t>S.NO.</t>
   </si>
@@ -845,6 +842,24 @@
     <t xml:space="preserve">Data Explorer </t>
   </si>
   <si>
+    <t xml:space="preserve">  ☐ Faceted search - Numeric fields in faceted search are displayed as a slider @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Text fields in faceted search are displayed as checkboxes @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Filters can be organized in multiple tabs @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Display names can be set for the filters @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Data shown in charts corresponds to filters set @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Faceted search - Nested data - Nested fields can be shown @manual</t>
+  </si>
+  <si>
     <t>SUITE 35</t>
   </si>
   <si>
@@ -1299,36 +1314,39 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>SUITES</t>
+  </si>
+  <si>
+    <t>TESTS</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1694,24 +1712,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G376"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A376" sqref="A376"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="195" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-  </cols>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G382"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1734,7 +1739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1742,7 +1747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1753,7 +1758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1764,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1775,7 +1780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1786,7 +1791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1805,7 +1810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1816,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1827,7 +1832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1835,7 +1840,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1846,7 +1851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1857,7 +1862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1865,7 +1870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>10</v>
       </c>
@@ -1876,7 +1881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>11</v>
       </c>
@@ -1887,7 +1892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>12</v>
       </c>
@@ -1898,7 +1903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1906,7 +1911,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>13</v>
       </c>
@@ -1923,7 +1928,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -1940,7 +1945,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>15</v>
       </c>
@@ -1957,7 +1962,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>16</v>
       </c>
@@ -1974,7 +1979,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>17</v>
       </c>
@@ -1991,7 +1996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>18</v>
       </c>
@@ -2008,7 +2013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>19</v>
       </c>
@@ -2025,7 +2030,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>20</v>
       </c>
@@ -2042,7 +2047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>21</v>
       </c>
@@ -2059,7 +2064,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>22</v>
       </c>
@@ -2076,7 +2081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>23</v>
       </c>
@@ -2093,7 +2098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>24</v>
       </c>
@@ -2110,7 +2115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>25</v>
       </c>
@@ -2127,7 +2132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>26</v>
       </c>
@@ -2144,7 +2149,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>27</v>
       </c>
@@ -2161,7 +2166,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>28</v>
       </c>
@@ -2178,7 +2183,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>29</v>
       </c>
@@ -2197,7 +2202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>30</v>
       </c>
@@ -2208,7 +2213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>31</v>
       </c>
@@ -2219,7 +2224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>32</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>33</v>
       </c>
@@ -2241,7 +2246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>34</v>
       </c>
@@ -2252,7 +2257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>35</v>
       </c>
@@ -2263,7 +2268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>36</v>
       </c>
@@ -2274,7 +2279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>37</v>
       </c>
@@ -2285,7 +2290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>38</v>
       </c>
@@ -2296,7 +2301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>39</v>
       </c>
@@ -2307,7 +2312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>40</v>
       </c>
@@ -2318,7 +2323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>41</v>
       </c>
@@ -2329,7 +2334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>42</v>
       </c>
@@ -2340,7 +2345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>43</v>
       </c>
@@ -2351,7 +2356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>44</v>
       </c>
@@ -2362,7 +2367,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>45</v>
       </c>
@@ -2373,7 +2378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>46</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>47</v>
       </c>
@@ -2395,7 +2400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>48</v>
       </c>
@@ -2406,7 +2411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>49</v>
       </c>
@@ -2417,7 +2422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>71</v>
       </c>
@@ -2425,7 +2430,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>50</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>51</v>
       </c>
@@ -2459,7 +2464,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>52</v>
       </c>
@@ -2476,7 +2481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>53</v>
       </c>
@@ -2493,7 +2498,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>54</v>
       </c>
@@ -2510,7 +2515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>55</v>
       </c>
@@ -2527,7 +2532,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>56</v>
       </c>
@@ -2544,7 +2549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>57</v>
       </c>
@@ -2561,7 +2566,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>81</v>
       </c>
@@ -2569,7 +2574,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>58</v>
       </c>
@@ -2586,7 +2591,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>59</v>
       </c>
@@ -2603,7 +2608,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>60</v>
       </c>
@@ -2620,7 +2625,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>61</v>
       </c>
@@ -2637,7 +2642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>87</v>
       </c>
@@ -2645,7 +2650,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>62</v>
       </c>
@@ -2656,7 +2661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>63</v>
       </c>
@@ -2667,7 +2672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>64</v>
       </c>
@@ -2678,7 +2683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>65</v>
       </c>
@@ -2689,7 +2694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>66</v>
       </c>
@@ -2700,7 +2705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>67</v>
       </c>
@@ -2711,7 +2716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>68</v>
       </c>
@@ -2722,7 +2727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>69</v>
       </c>
@@ -2733,7 +2738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -2741,7 +2746,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>70</v>
       </c>
@@ -2752,7 +2757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>71</v>
       </c>
@@ -2763,7 +2768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>72</v>
       </c>
@@ -2774,7 +2779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>101</v>
       </c>
@@ -2782,7 +2787,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>73</v>
       </c>
@@ -2799,7 +2804,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>74</v>
       </c>
@@ -2816,7 +2821,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>75</v>
       </c>
@@ -2833,7 +2838,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>76</v>
       </c>
@@ -2850,7 +2855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>77</v>
       </c>
@@ -2867,7 +2872,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>108</v>
       </c>
@@ -2875,7 +2880,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>78</v>
       </c>
@@ -2892,7 +2897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>79</v>
       </c>
@@ -2909,7 +2914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>112</v>
       </c>
@@ -2917,7 +2922,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>80</v>
       </c>
@@ -2934,7 +2939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>115</v>
       </c>
@@ -2942,7 +2947,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>81</v>
       </c>
@@ -2959,7 +2964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>82</v>
       </c>
@@ -2976,7 +2981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>83</v>
       </c>
@@ -2993,7 +2998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>84</v>
       </c>
@@ -3010,7 +3015,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>85</v>
       </c>
@@ -3027,7 +3032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>86</v>
       </c>
@@ -3044,7 +3049,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>87</v>
       </c>
@@ -3061,7 +3066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>124</v>
       </c>
@@ -3069,7 +3074,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>88</v>
       </c>
@@ -3086,7 +3091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>89</v>
       </c>
@@ -3103,7 +3108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>90</v>
       </c>
@@ -3120,7 +3125,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>91</v>
       </c>
@@ -3137,7 +3142,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>92</v>
       </c>
@@ -3154,7 +3159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>93</v>
       </c>
@@ -3171,7 +3176,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>94</v>
       </c>
@@ -3188,7 +3193,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>95</v>
       </c>
@@ -3205,7 +3210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>96</v>
       </c>
@@ -3222,7 +3227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="113" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>97</v>
       </c>
@@ -3239,7 +3244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>98</v>
       </c>
@@ -3256,7 +3261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>99</v>
       </c>
@@ -3273,7 +3278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>100</v>
       </c>
@@ -3290,7 +3295,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>101</v>
       </c>
@@ -3307,7 +3312,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>102</v>
       </c>
@@ -3324,7 +3329,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>141</v>
       </c>
@@ -3332,7 +3337,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="120" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>103</v>
       </c>
@@ -3349,7 +3354,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>104</v>
       </c>
@@ -3366,7 +3371,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>105</v>
       </c>
@@ -3383,7 +3388,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>106</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>107</v>
       </c>
@@ -3417,7 +3422,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>108</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="126" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>109</v>
       </c>
@@ -3451,7 +3456,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="127" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>150</v>
       </c>
@@ -3459,7 +3464,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="128" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>110</v>
       </c>
@@ -3476,7 +3481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="129" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>111</v>
       </c>
@@ -3493,7 +3498,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>112</v>
       </c>
@@ -3510,7 +3515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>113</v>
       </c>
@@ -3527,7 +3532,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="132" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>114</v>
       </c>
@@ -3544,7 +3549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>157</v>
       </c>
@@ -3552,7 +3557,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>115</v>
       </c>
@@ -3563,7 +3568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>116</v>
       </c>
@@ -3574,7 +3579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>117</v>
       </c>
@@ -3585,7 +3590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>118</v>
       </c>
@@ -3596,7 +3601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>119</v>
       </c>
@@ -3607,7 +3612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>120</v>
       </c>
@@ -3618,7 +3623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>121</v>
       </c>
@@ -3629,7 +3634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>122</v>
       </c>
@@ -3640,7 +3645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>123</v>
       </c>
@@ -3651,7 +3656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>124</v>
       </c>
@@ -3662,7 +3667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>125</v>
       </c>
@@ -3673,7 +3678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>170</v>
       </c>
@@ -3681,7 +3686,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="146" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>126</v>
       </c>
@@ -3692,7 +3697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>127</v>
       </c>
@@ -3703,7 +3708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>128</v>
       </c>
@@ -3714,7 +3719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>129</v>
       </c>
@@ -3725,7 +3730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>130</v>
       </c>
@@ -3736,7 +3741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>131</v>
       </c>
@@ -3747,7 +3752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>132</v>
       </c>
@@ -3758,7 +3763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>179</v>
       </c>
@@ -3766,7 +3771,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="154" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>133</v>
       </c>
@@ -3777,7 +3782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>134</v>
       </c>
@@ -3788,7 +3793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>183</v>
       </c>
@@ -3796,7 +3801,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="157" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>135</v>
       </c>
@@ -3813,7 +3818,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="158" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>186</v>
       </c>
@@ -3821,7 +3826,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="159" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>136</v>
       </c>
@@ -3832,7 +3837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>137</v>
       </c>
@@ -3843,7 +3848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>138</v>
       </c>
@@ -3854,7 +3859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>139</v>
       </c>
@@ -3865,7 +3870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>140</v>
       </c>
@@ -3876,7 +3881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>141</v>
       </c>
@@ -3887,7 +3892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>142</v>
       </c>
@@ -3898,7 +3903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>143</v>
       </c>
@@ -3909,7 +3914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>144</v>
       </c>
@@ -3920,7 +3925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>193</v>
       </c>
@@ -3928,7 +3933,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="169" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>145</v>
       </c>
@@ -3945,7 +3950,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="170" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>146</v>
       </c>
@@ -3962,7 +3967,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="171" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>147</v>
       </c>
@@ -3979,7 +3984,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="172" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>198</v>
       </c>
@@ -3987,7 +3992,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="173" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>148</v>
       </c>
@@ -4004,7 +4009,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="174" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>149</v>
       </c>
@@ -4021,7 +4026,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="175" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>150</v>
       </c>
@@ -4038,7 +4043,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="176" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>151</v>
       </c>
@@ -4055,7 +4060,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="177" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>152</v>
       </c>
@@ -4072,7 +4077,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="178" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>205</v>
       </c>
@@ -4080,7 +4085,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="179" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>153</v>
       </c>
@@ -4097,7 +4102,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="180" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>154</v>
       </c>
@@ -4114,7 +4119,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="181" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>155</v>
       </c>
@@ -4131,7 +4136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>156</v>
       </c>
@@ -4148,7 +4153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="183" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>157</v>
       </c>
@@ -4165,7 +4170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>212</v>
       </c>
@@ -4173,7 +4178,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="185" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>158</v>
       </c>
@@ -4190,7 +4195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>159</v>
       </c>
@@ -4207,7 +4212,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="187" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>160</v>
       </c>
@@ -4224,7 +4229,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>161</v>
       </c>
@@ -4241,7 +4246,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="189" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>162</v>
       </c>
@@ -4258,7 +4263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="190" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>163</v>
       </c>
@@ -4275,7 +4280,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="191" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>164</v>
       </c>
@@ -4292,7 +4297,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="192" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>165</v>
       </c>
@@ -4309,7 +4314,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="193" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>166</v>
       </c>
@@ -4326,7 +4331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="194" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>167</v>
       </c>
@@ -4343,7 +4348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>168</v>
       </c>
@@ -4360,7 +4365,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="196" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>169</v>
       </c>
@@ -4377,7 +4382,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="197" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>170</v>
       </c>
@@ -4394,7 +4399,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="198" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>171</v>
       </c>
@@ -4411,7 +4416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="199" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>172</v>
       </c>
@@ -4428,7 +4433,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="200" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>173</v>
       </c>
@@ -4445,7 +4450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="201" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>174</v>
       </c>
@@ -4462,7 +4467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="202" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>175</v>
       </c>
@@ -4479,7 +4484,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="203" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>232</v>
       </c>
@@ -4487,7 +4492,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="204" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>176</v>
       </c>
@@ -4504,7 +4509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="205" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>177</v>
       </c>
@@ -4521,7 +4526,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="206" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>178</v>
       </c>
@@ -4538,7 +4543,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="207" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>179</v>
       </c>
@@ -4555,7 +4560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="208" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>180</v>
       </c>
@@ -4572,7 +4577,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="209" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>181</v>
       </c>
@@ -4589,7 +4594,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="210" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>182</v>
       </c>
@@ -4606,7 +4611,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="211" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>241</v>
       </c>
@@ -4614,7 +4619,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="212" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>183</v>
       </c>
@@ -4625,7 +4630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>184</v>
       </c>
@@ -4636,7 +4641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>185</v>
       </c>
@@ -4647,7 +4652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>186</v>
       </c>
@@ -4658,7 +4663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>187</v>
       </c>
@@ -4669,7 +4674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>248</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="218" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>188</v>
       </c>
@@ -4688,7 +4693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>189</v>
       </c>
@@ -4699,7 +4704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>190</v>
       </c>
@@ -4710,7 +4715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>191</v>
       </c>
@@ -4721,7 +4726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>192</v>
       </c>
@@ -4732,7 +4737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>254</v>
       </c>
@@ -4740,7 +4745,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="224" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>193</v>
       </c>
@@ -4751,7 +4756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>194</v>
       </c>
@@ -4762,7 +4767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>195</v>
       </c>
@@ -4773,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>259</v>
       </c>
@@ -4781,7 +4786,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="228" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>196</v>
       </c>
@@ -4798,7 +4803,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="229" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>197</v>
       </c>
@@ -4815,7 +4820,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="230" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3">
         <v>198</v>
       </c>
@@ -4832,7 +4837,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="231" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>264</v>
       </c>
@@ -4840,7 +4845,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="232" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>199</v>
       </c>
@@ -4857,7 +4862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="233" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>267</v>
       </c>
@@ -4865,7 +4870,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="234" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>200</v>
       </c>
@@ -4876,7 +4881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>201</v>
       </c>
@@ -4887,7 +4892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>202</v>
       </c>
@@ -4898,7 +4903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>203</v>
       </c>
@@ -4909,7 +4914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>204</v>
       </c>
@@ -4920,7 +4925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="239" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>274</v>
       </c>
@@ -4928,484 +4933,484 @@
         <v>275</v>
       </c>
     </row>
-    <row r="240" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A240" s="2" t="s">
+    <row r="240" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="3">
+        <v>205</v>
+      </c>
+      <c r="B240" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="C240" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="3">
+        <v>206</v>
+      </c>
+      <c r="B241" s="3" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="241" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A241" s="3">
-        <v>205</v>
-      </c>
-      <c r="B241" s="3" t="s">
+      <c r="C241" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="3">
+        <v>207</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C241" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E241" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F241" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A242" s="3">
-        <v>206</v>
-      </c>
-      <c r="B242" s="3" t="s">
+      <c r="C242" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="3">
+        <v>208</v>
+      </c>
+      <c r="B243" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C242" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E242" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F242" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A243" s="3">
-        <v>207</v>
-      </c>
-      <c r="B243" s="3" t="s">
+      <c r="C243" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="3">
+        <v>209</v>
+      </c>
+      <c r="B244" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C243" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
+      <c r="C244" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="3">
+        <v>210</v>
+      </c>
+      <c r="B245" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="C245" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A245" s="3">
-        <v>208</v>
-      </c>
-      <c r="B245" s="3" t="s">
+      <c r="B246" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C245" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A246" s="3">
-        <v>209</v>
-      </c>
-      <c r="B246" s="3" t="s">
+    </row>
+    <row r="247" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="3">
+        <v>211</v>
+      </c>
+      <c r="B247" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C246" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A247" s="3">
-        <v>210</v>
-      </c>
-      <c r="B247" s="3" t="s">
+      <c r="C247" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F247" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="3">
+        <v>212</v>
+      </c>
+      <c r="B248" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C247" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A248" s="3">
-        <v>211</v>
-      </c>
-      <c r="B248" s="3" t="s">
+      <c r="C248" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="3">
+        <v>213</v>
+      </c>
+      <c r="B249" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C248" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
+      <c r="C249" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B249" s="2" t="s">
+      <c r="B250" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="250" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A250" s="3">
-        <v>212</v>
-      </c>
-      <c r="B250" s="3" t="s">
+    <row r="251" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="3">
+        <v>214</v>
+      </c>
+      <c r="B251" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C250" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A251" s="3">
-        <v>213</v>
-      </c>
-      <c r="B251" s="3" t="s">
+      <c r="C251" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="3">
+        <v>215</v>
+      </c>
+      <c r="B252" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A252" s="3">
-        <v>214</v>
-      </c>
-      <c r="B252" s="3" t="s">
+      <c r="C252" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="3">
+        <v>216</v>
+      </c>
+      <c r="B253" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C252" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A253" s="3">
-        <v>215</v>
-      </c>
-      <c r="B253" s="3" t="s">
+      <c r="C253" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="3">
+        <v>217</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="C253" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A254" s="3">
-        <v>216</v>
-      </c>
-      <c r="B254" s="3" t="s">
+      <c r="C254" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C254" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A255" s="3">
-        <v>217</v>
-      </c>
-      <c r="B255" s="3" t="s">
+      <c r="B255" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C255" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A256" s="2" t="s">
+    </row>
+    <row r="256" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="3">
+        <v>218</v>
+      </c>
+      <c r="B256" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B256" s="2" t="s">
+      <c r="C256" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="3">
+        <v>219</v>
+      </c>
+      <c r="B257" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A257" s="3">
-        <v>218</v>
-      </c>
-      <c r="B257" s="3" t="s">
+      <c r="C257" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="3">
+        <v>220</v>
+      </c>
+      <c r="B258" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C257" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A258" s="3">
-        <v>219</v>
-      </c>
-      <c r="B258" s="3" t="s">
+      <c r="C258" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="3">
+        <v>221</v>
+      </c>
+      <c r="B259" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="C258" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A259" s="3">
-        <v>220</v>
-      </c>
-      <c r="B259" s="3" t="s">
+      <c r="C259" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="3">
+        <v>222</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C259" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A260" s="3">
-        <v>221</v>
-      </c>
-      <c r="B260" s="3" t="s">
+      <c r="C260" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="3">
+        <v>223</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C260" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A261" s="3">
-        <v>222</v>
-      </c>
-      <c r="B261" s="3" t="s">
+      <c r="C261" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C261" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
+      <c r="B262" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B262" s="2" t="s">
+    </row>
+    <row r="263" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="3">
+        <v>224</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A263" s="3">
-        <v>223</v>
-      </c>
-      <c r="B263" s="3" t="s">
+      <c r="C263" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="3">
+        <v>225</v>
+      </c>
+      <c r="B264" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="C263" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E263" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F263" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A264" s="3">
-        <v>224</v>
-      </c>
-      <c r="B264" s="3" t="s">
+      <c r="C264" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="3">
+        <v>226</v>
+      </c>
+      <c r="B265" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="C264" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E264" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F264" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A265" s="2" t="s">
+      <c r="C265" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="3">
+        <v>227</v>
+      </c>
+      <c r="B266" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B265" s="2" t="s">
+      <c r="C266" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="3">
+        <v>228</v>
+      </c>
+      <c r="B267" s="3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A266" s="3">
-        <v>225</v>
-      </c>
-      <c r="B266" s="3" t="s">
+      <c r="C267" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C266" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E266" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F266" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A267" s="3">
-        <v>226</v>
-      </c>
-      <c r="B267" s="3" t="s">
+      <c r="B268" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C267" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E267" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F267" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A268" s="2" t="s">
+    </row>
+    <row r="269" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="3">
+        <v>229</v>
+      </c>
+      <c r="B269" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B268" s="2" t="s">
+      <c r="C269" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E269" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F269" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="3">
+        <v>230</v>
+      </c>
+      <c r="B270" s="3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="269" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A269" s="3">
-        <v>227</v>
-      </c>
-      <c r="B269" s="3" t="s">
+      <c r="C270" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E270" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F270" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C269" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E269" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F269" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A270" s="2" t="s">
+      <c r="B271" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B270" s="2" t="s">
+    </row>
+    <row r="272" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="3">
+        <v>231</v>
+      </c>
+      <c r="B272" s="3" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="271" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A271" s="3">
-        <v>228</v>
-      </c>
-      <c r="B271" s="3" t="s">
+      <c r="C272" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E272" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F272" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="3">
+        <v>232</v>
+      </c>
+      <c r="B273" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C271" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A272" s="3">
-        <v>229</v>
-      </c>
-      <c r="B272" s="3" t="s">
+      <c r="C273" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E273" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F273" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C272" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A273" s="3">
-        <v>230</v>
-      </c>
-      <c r="B273" s="3" t="s">
+      <c r="B274" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C273" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A274" s="3">
-        <v>231</v>
-      </c>
-      <c r="B274" s="3" t="s">
+    </row>
+    <row r="275" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="3">
+        <v>233</v>
+      </c>
+      <c r="B275" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="C274" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A275" s="2" t="s">
+      <c r="C275" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E275" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F275" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B275" s="2" t="s">
+      <c r="B276" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="276" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A276" s="3">
-        <v>232</v>
-      </c>
-      <c r="B276" s="3" t="s">
+    <row r="277" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="3">
+        <v>234</v>
+      </c>
+      <c r="B277" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C276" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A277" s="3">
-        <v>233</v>
-      </c>
-      <c r="B277" s="3" t="s">
+      <c r="C277" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="3">
+        <v>235</v>
+      </c>
+      <c r="B278" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="C277" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A278" s="3">
-        <v>234</v>
-      </c>
-      <c r="B278" s="3" t="s">
+      <c r="C278" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="3">
+        <v>236</v>
+      </c>
+      <c r="B279" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C278" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A279" s="3">
-        <v>235</v>
-      </c>
-      <c r="B279" s="3" t="s">
+      <c r="C279" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="3">
+        <v>237</v>
+      </c>
+      <c r="B280" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="C279" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A280" s="3">
-        <v>236</v>
-      </c>
-      <c r="B280" s="3" t="s">
+      <c r="C280" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C280" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A281" s="3">
-        <v>237</v>
-      </c>
-      <c r="B281" s="3" t="s">
+      <c r="B281" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C281" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="282" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A282" s="3">
         <v>238</v>
       </c>
@@ -5416,7 +5421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A283" s="3">
         <v>239</v>
       </c>
@@ -5427,7 +5432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A284" s="3">
         <v>240</v>
       </c>
@@ -5438,7 +5443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A285" s="3">
         <v>241</v>
       </c>
@@ -5449,7 +5454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A286" s="3">
         <v>242</v>
       </c>
@@ -5460,7 +5465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A287" s="3">
         <v>243</v>
       </c>
@@ -5471,7 +5476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="288" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="3">
         <v>244</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="289" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" s="3">
         <v>245</v>
       </c>
@@ -5493,152 +5498,155 @@
         <v>10</v>
       </c>
     </row>
-    <row r="290" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A290" s="2" t="s">
+    <row r="290" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="3">
+        <v>246</v>
+      </c>
+      <c r="B290" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="B290" s="2" t="s">
+      <c r="C290" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="3">
+        <v>247</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A291" s="3">
-        <v>246</v>
-      </c>
-      <c r="B291" s="3" t="s">
+      <c r="C291" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="3">
+        <v>248</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C291" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A292" s="3">
-        <v>247</v>
-      </c>
-      <c r="B292" s="3" t="s">
+      <c r="C292" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="3">
+        <v>249</v>
+      </c>
+      <c r="B293" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="C292" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A293" s="3">
-        <v>248</v>
-      </c>
-      <c r="B293" s="3" t="s">
+      <c r="C293" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="3">
+        <v>250</v>
+      </c>
+      <c r="B294" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C293" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A294" s="2" t="s">
+      <c r="C294" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="3">
+        <v>251</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="B294" s="2" t="s">
+      <c r="C295" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A295" s="3">
-        <v>249</v>
-      </c>
-      <c r="B295" s="3" t="s">
+      <c r="B296" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C295" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A296" s="3">
-        <v>250</v>
-      </c>
-      <c r="B296" s="3" t="s">
+    </row>
+    <row r="297" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="3">
+        <v>252</v>
+      </c>
+      <c r="B297" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="C296" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A297" s="3">
-        <v>251</v>
-      </c>
-      <c r="B297" s="3" t="s">
+      <c r="C297" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="3">
+        <v>253</v>
+      </c>
+      <c r="B298" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="C297" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A298" s="2" t="s">
+      <c r="C298" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="3">
+        <v>254</v>
+      </c>
+      <c r="B299" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="B298" s="2" t="s">
+      <c r="C299" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A299" s="3">
-        <v>252</v>
-      </c>
-      <c r="B299" s="3" t="s">
+      <c r="B300" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="C299" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A300" s="3">
-        <v>253</v>
-      </c>
-      <c r="B300" s="3" t="s">
+    </row>
+    <row r="301" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="3">
+        <v>255</v>
+      </c>
+      <c r="B301" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="C300" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A301" s="3">
-        <v>254</v>
-      </c>
-      <c r="B301" s="3" t="s">
+      <c r="C301" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="3">
+        <v>256</v>
+      </c>
+      <c r="B302" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="C301" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A302" s="3">
-        <v>255</v>
-      </c>
-      <c r="B302" s="3" t="s">
+      <c r="C302" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="3">
+        <v>257</v>
+      </c>
+      <c r="B303" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="C302" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A303" s="3">
-        <v>256</v>
-      </c>
-      <c r="B303" s="3" t="s">
-        <v>349</v>
-      </c>
       <c r="C303" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>351</v>
       </c>
@@ -5646,9 +5654,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="305" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B305" s="3" t="s">
         <v>353</v>
@@ -5657,9 +5665,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A306" s="3">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B306" s="3" t="s">
         <v>354</v>
@@ -5668,9 +5676,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A307" s="3">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B307" s="3" t="s">
         <v>355</v>
@@ -5679,9 +5687,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A308" s="3">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B308" s="3" t="s">
         <v>356</v>
@@ -5690,29 +5698,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="309" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A309" s="3">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B309" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C309" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A310" s="3">
-        <v>262</v>
-      </c>
-      <c r="B310" s="3" t="s">
+      <c r="B310" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C310" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="311" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A311" s="3">
         <v>263</v>
       </c>
@@ -5723,7 +5728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A312" s="3">
         <v>264</v>
       </c>
@@ -5734,83 +5739,86 @@
         <v>10</v>
       </c>
     </row>
-    <row r="313" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A313" s="3">
         <v>265</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="314" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" s="3">
         <v>266</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="315" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A315" s="3">
         <v>267</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A316" s="3">
         <v>268</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="317" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3">
         <v>269</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="318" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A318" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B318" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A318" s="3">
+        <v>270</v>
+      </c>
+      <c r="B318" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C318" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" s="3">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="320" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" s="3">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B320" s="3" t="s">
         <v>366</v>
@@ -5819,9 +5827,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="321" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" s="3">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B321" s="3" t="s">
         <v>367</v>
@@ -5830,9 +5838,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="322" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="3">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B322" s="3" t="s">
         <v>368</v>
@@ -5841,300 +5849,261 @@
         <v>10</v>
       </c>
     </row>
-    <row r="323" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B323" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C323" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C323" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A324" s="2" t="s">
+      <c r="B324" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B324" s="2" t="s">
+    </row>
+    <row r="325" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A325" s="3">
+        <v>276</v>
+      </c>
+      <c r="B325" s="3" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A325" s="3">
-        <v>275</v>
-      </c>
-      <c r="B325" s="3" t="s">
+      <c r="C325" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A326" s="3">
+        <v>277</v>
+      </c>
+      <c r="B326" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C326" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A327" s="3">
+        <v>278</v>
+      </c>
+      <c r="B327" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C327" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A328" s="3">
+        <v>279</v>
+      </c>
+      <c r="B328" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C328" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A329" s="3">
+        <v>280</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C329" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A330" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A331" s="3">
+        <v>281</v>
+      </c>
+      <c r="B331" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C325" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A326" s="3">
-        <v>276</v>
-      </c>
-      <c r="B326" s="3" t="s">
+      <c r="C331" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A332" s="3">
+        <v>282</v>
+      </c>
+      <c r="B332" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C326" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A327" s="3">
-        <v>277</v>
-      </c>
-      <c r="B327" s="3" t="s">
+      <c r="C332" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="3">
+        <v>283</v>
+      </c>
+      <c r="B333" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C327" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A328" s="3">
-        <v>278</v>
-      </c>
-      <c r="B328" s="3" t="s">
+      <c r="C333" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="3">
+        <v>284</v>
+      </c>
+      <c r="B334" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C328" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A329" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="B329" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A330" s="3">
-        <v>279</v>
-      </c>
-      <c r="B330" s="3" t="s">
+      <c r="C334" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="3">
+        <v>285</v>
+      </c>
+      <c r="B336" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C330" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="331" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A331" s="3">
-        <v>280</v>
-      </c>
-      <c r="B331" s="3" t="s">
+      <c r="C336" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="3">
+        <v>286</v>
+      </c>
+      <c r="B337" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C331" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="332" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A332" s="3">
-        <v>281</v>
-      </c>
-      <c r="B332" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="C332" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="333" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A333" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="B333" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="334" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A334" s="3">
-        <v>282</v>
-      </c>
-      <c r="B334" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="C334" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="335" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A335" s="3">
-        <v>283</v>
-      </c>
-      <c r="B335" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="C335" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A336" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="B336" s="2" t="s">
+      <c r="C337" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="3">
+        <v>287</v>
+      </c>
+      <c r="B338" s="3" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="337" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A337" s="2" t="s">
+      <c r="C338" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B337" s="2" t="s">
+      <c r="B339" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="338" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A338" s="3">
-        <v>284</v>
-      </c>
-      <c r="B338" s="3" t="s">
+    <row r="340" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="3">
+        <v>288</v>
+      </c>
+      <c r="B340" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="C338" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E338" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F338" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="339" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A339" s="2" t="s">
+      <c r="C340" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="3">
+        <v>289</v>
+      </c>
+      <c r="B341" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="B339" s="2" t="s">
+      <c r="C341" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="2" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="340" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A340" s="2" t="s">
+      <c r="B342" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B340" s="2" t="s">
+    </row>
+    <row r="343" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="341" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A341" s="2" t="s">
+      <c r="B343" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B341" s="2" t="s">
+    </row>
+    <row r="344" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="3">
+        <v>290</v>
+      </c>
+      <c r="B344" s="3" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="342" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A342" s="3">
-        <v>285</v>
-      </c>
-      <c r="B342" s="3" t="s">
+      <c r="C344" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E344" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F344" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C342" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E342" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F342" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="343" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A343" s="3">
-        <v>286</v>
-      </c>
-      <c r="B343" s="3" t="s">
+      <c r="B345" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="C343" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E343" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F343" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="344" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A344" s="3">
-        <v>287</v>
-      </c>
-      <c r="B344" s="3" t="s">
+    </row>
+    <row r="346" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="C344" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E344" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F344" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="345" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A345" s="3">
-        <v>288</v>
-      </c>
-      <c r="B345" s="3" t="s">
+      <c r="B346" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="C345" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E345" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F345" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="346" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A346" s="3">
-        <v>289</v>
-      </c>
-      <c r="B346" s="3" t="s">
+    </row>
+    <row r="347" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C346" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E346" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F346" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="347" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A347" s="3">
-        <v>290</v>
-      </c>
-      <c r="B347" s="3" t="s">
+      <c r="B347" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="C347" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E347" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F347" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="348" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="348" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3">
         <v>291</v>
       </c>
@@ -6151,7 +6120,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="349" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A349" s="3">
         <v>292</v>
       </c>
@@ -6168,7 +6137,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="350" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3">
         <v>293</v>
       </c>
@@ -6185,7 +6154,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="351" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3">
         <v>294</v>
       </c>
@@ -6202,7 +6171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="352" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3">
         <v>295</v>
       </c>
@@ -6219,7 +6188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="353" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A353" s="3">
         <v>296</v>
       </c>
@@ -6236,7 +6205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="354" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A354" s="3">
         <v>297</v>
       </c>
@@ -6253,7 +6222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="355" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A355" s="3">
         <v>298</v>
       </c>
@@ -6270,140 +6239,176 @@
         <v>33</v>
       </c>
     </row>
-    <row r="356" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A356" s="2" t="s">
+    <row r="356" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="3">
+        <v>299</v>
+      </c>
+      <c r="B356" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="B356" s="2" t="s">
+      <c r="C356" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E356" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F356" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A357" s="3">
+        <v>300</v>
+      </c>
+      <c r="B357" s="3" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="357" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A357" s="3">
-        <v>299</v>
-      </c>
-      <c r="B357" s="3" t="s">
+      <c r="C357" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E357" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F357" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="3">
+        <v>301</v>
+      </c>
+      <c r="B358" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="C357" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E357" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F357" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="358" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A358" s="3">
-        <v>300</v>
-      </c>
-      <c r="B358" s="3" t="s">
+      <c r="C358" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E358" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F358" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A359" s="3">
+        <v>302</v>
+      </c>
+      <c r="B359" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C358" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E358" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F358" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="359" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A359" s="3">
-        <v>301</v>
-      </c>
-      <c r="B359" s="3" t="s">
+      <c r="C359" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E359" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F359" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A360" s="3">
+        <v>303</v>
+      </c>
+      <c r="B360" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="C359" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E359" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F359" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="360" spans="1:6" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A360" s="2" t="s">
+      <c r="C360" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E360" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F360" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="3">
+        <v>304</v>
+      </c>
+      <c r="B361" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="B360" s="2" t="s">
+      <c r="C361" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E361" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F361" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="2" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="361" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A361" s="3">
-        <v>302</v>
-      </c>
-      <c r="B361" s="3" t="s">
+      <c r="B362" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="C361" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A362" s="3">
-        <v>303</v>
-      </c>
-      <c r="B362" s="3" t="s">
+    </row>
+    <row r="363" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="3">
+        <v>305</v>
+      </c>
+      <c r="B363" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="C362" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="363" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A363" s="3">
-        <v>304</v>
-      </c>
-      <c r="B363" s="3" t="s">
+      <c r="C363" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E363" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F363" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="3">
+        <v>306</v>
+      </c>
+      <c r="B364" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="C363" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="364" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A364" s="3">
-        <v>305</v>
-      </c>
-      <c r="B364" s="3" t="s">
+      <c r="C364" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E364" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F364" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A365" s="3">
+        <v>307</v>
+      </c>
+      <c r="B365" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="C364" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="365" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A365" s="3">
-        <v>306</v>
-      </c>
-      <c r="B365" s="3" t="s">
+      <c r="C365" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E365" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F365" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C365" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="366" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A366" s="3">
-        <v>307</v>
-      </c>
-      <c r="B366" s="3" t="s">
+      <c r="B366" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C366" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="367" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="367" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A367" s="3">
         <v>308</v>
       </c>
@@ -6414,7 +6419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="368" spans="1:6" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A368" s="3">
         <v>309</v>
       </c>
@@ -6425,7 +6430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="369" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A369" s="3">
         <v>310</v>
       </c>
@@ -6436,7 +6441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="370" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A370" s="3">
         <v>311</v>
       </c>
@@ -6447,7 +6452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="371" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A371" s="3">
         <v>312</v>
       </c>
@@ -6458,7 +6463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="372" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A372" s="3">
         <v>313</v>
       </c>
@@ -6469,7 +6474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="373" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A373" s="3">
         <v>314</v>
       </c>
@@ -6480,7 +6485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="374" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A374" s="3">
         <v>315</v>
       </c>
@@ -6491,7 +6496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="375" spans="1:3" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3">
         <v>316</v>
       </c>
@@ -6502,16 +6507,125 @@
         <v>10</v>
       </c>
     </row>
-    <row r="376" spans="1:3" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A376" s="2" t="s">
+    <row r="376" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A376" s="3">
+        <v>317</v>
+      </c>
+      <c r="B376" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="B376" s="2" t="s">
+      <c r="C376" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A377" s="3">
+        <v>318</v>
+      </c>
+      <c r="B377" s="3" t="s">
         <v>427</v>
+      </c>
+      <c r="C377" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A378" s="3">
+        <v>319</v>
+      </c>
+      <c r="B378" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C378" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A379" s="3">
+        <v>320</v>
+      </c>
+      <c r="B379" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C379" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A380" s="3">
+        <v>321</v>
+      </c>
+      <c r="B380" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C380" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A381" s="3">
+        <v>322</v>
+      </c>
+      <c r="B381" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C381" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
disabling screenshots and updating test plan
</commit_message>
<xml_diff>
--- a/test-plan.xlsx
+++ b/test-plan.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="444">
   <si>
     <t>S.NO.</t>
   </si>
@@ -809,13 +809,25 @@
     <t>SUITE 32</t>
   </si>
   <si>
+    <t xml:space="preserve">Redirect invalid urls to 404 page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Valid urls are not redirected to 404 page @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Invalid urls get redirected to 404 page @manual</t>
+  </si>
+  <si>
+    <t>SUITE 33</t>
+  </si>
+  <si>
     <t xml:space="preserve">CoreMetadataPageTest </t>
   </si>
   <si>
     <t xml:space="preserve">  ☐ test core metadata page @coreMetadataPage @portal</t>
   </si>
   <si>
-    <t>SUITE 33</t>
+    <t>SUITE 34</t>
   </si>
   <si>
     <t xml:space="preserve">DashboardReports - https://ctds-planx.atlassian.net/browse/PXP-4252 </t>
@@ -836,7 +848,7 @@
     <t xml:space="preserve">  ☐ The dashboard reports gracefully handle no data @manual</t>
   </si>
   <si>
-    <t>SUITE 34</t>
+    <t>SUITE 35</t>
   </si>
   <si>
     <t xml:space="preserve">Data Explorer </t>
@@ -860,7 +872,13 @@
     <t xml:space="preserve">  ☐ Faceted search - Nested data - Nested fields can be shown @manual</t>
   </si>
   <si>
-    <t>SUITE 35</t>
+    <t xml:space="preserve">  ☐ Table - Data displayed in the table is correct @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Table - Nested data displayed in the table is correct @manual</t>
+  </si>
+  <si>
+    <t>SUITE 36</t>
   </si>
   <si>
     <t xml:space="preserve">DataUploadTest </t>
@@ -875,7 +893,7 @@
     <t xml:space="preserve">  ☐ Upload clinical data file through portal large enough to trigger chunking @manual @regression</t>
   </si>
   <si>
-    <t>SUITE 36</t>
+    <t>SUITE 37</t>
   </si>
   <si>
     <t xml:space="preserve">ExportToWorkspaceTest </t>
@@ -893,7 +911,7 @@
     <t xml:space="preserve">  ☐ Export default manifest, mount it and check manifest name @exportToWorkspacePortalHatchery @portal @manual</t>
   </si>
   <si>
-    <t>SUITE 37</t>
+    <t>SUITE 38</t>
   </si>
   <si>
     <t xml:space="preserve">File Explorer - https://ctds-planx.atlassian.net/browse/PXP-4777 </t>
@@ -917,7 +935,7 @@
     <t xml:space="preserve">  ☐ Verify labels on the charts in File Explorer page @manual</t>
   </si>
   <si>
-    <t>SUITE 38</t>
+    <t>SUITE 39</t>
   </si>
   <si>
     <t xml:space="preserve">Homepage Chart Nodes </t>
@@ -938,7 +956,7 @@
     <t xml:space="preserve">  ☐ When Homepage Charts is disabled, logged-in users should see summary charts of ONLY the projects they have access to on the landing page @manual</t>
   </si>
   <si>
-    <t>SUITE 39</t>
+    <t>SUITE 40</t>
   </si>
   <si>
     <t xml:space="preserve">Homepage </t>
@@ -950,7 +968,7 @@
     <t xml:space="preserve">  ☐ login @portal @topBarLogin</t>
   </si>
   <si>
-    <t>SUITE 40</t>
+    <t>SUITE 41</t>
   </si>
   <si>
     <t xml:space="preserve">Indexing GUI </t>
@@ -962,7 +980,10 @@
     <t xml:space="preserve">  ☐ Navigate to the indexing page and download a full indexd manifest @indexing</t>
   </si>
   <si>
-    <t>SUITE 41</t>
+    <t xml:space="preserve">  ☐ Navigate to the indexing page and upload an invalid manifest @indexing</t>
+  </si>
+  <si>
+    <t>SUITE 42</t>
   </si>
   <si>
     <t xml:space="preserve">Login </t>
@@ -971,7 +992,7 @@
     <t xml:space="preserve">  ☐ Login redirects to requested page @loginRedirect</t>
   </si>
   <si>
-    <t>SUITE 42</t>
+    <t>SUITE 43</t>
   </si>
   <si>
     <t xml:space="preserve">Windmill configurable profile page </t>
@@ -989,7 +1010,7 @@
     <t xml:space="preserve">  ☐ When configuration has showArboristAuthzOnProfile: false, profile page does not show resources table from Arborist @manual</t>
   </si>
   <si>
-    <t>SUITE 43</t>
+    <t>SUITE 44</t>
   </si>
   <si>
     <t xml:space="preserve">RoleBasedUI - https://ctds-planx.atlassian.net/browse/PXP-4252 </t>
@@ -1037,7 +1058,7 @@
     <t xml:space="preserve">  ☐ The file page download button is not present if the user does not have read-storage permission on the file @manual</t>
   </si>
   <si>
-    <t>SUITE 44</t>
+    <t>SUITE 45</t>
   </si>
   <si>
     <t xml:space="preserve">Terra Export Warning Test Plan </t>
@@ -1052,7 +1073,7 @@
     <t xml:space="preserve">  ☐ When Terra Export Warning is DISABLED, user should NOT be warned when exporting N or more subjects @manual</t>
   </si>
   <si>
-    <t>SUITE 45</t>
+    <t>SUITE 46</t>
   </si>
   <si>
     <t xml:space="preserve">Tiered Access </t>
@@ -1067,7 +1088,7 @@
     <t xml:space="preserve">  ☐ Verify summary charts displayed correctly for partially authorized users @manual @regression @bugfix</t>
   </si>
   <si>
-    <t>SUITE 46</t>
+    <t>SUITE 47</t>
   </si>
   <si>
     <t xml:space="preserve">1. Linking accounts - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1085,7 +1106,7 @@
     <t xml:space="preserve">  ☐ Unlink Google identity from the NIH user @manual</t>
   </si>
   <si>
-    <t>SUITE 47</t>
+    <t>SUITE 48</t>
   </si>
   <si>
     <t xml:space="preserve">2. Service accounts registration - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1121,7 +1142,7 @@
     <t xml:space="preserve">  ☐ Delete existing service account @manual</t>
   </si>
   <si>
-    <t>SUITE 48</t>
+    <t>SUITE 49</t>
   </si>
   <si>
     <t xml:space="preserve">3. Google Credentials - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1142,13 +1163,13 @@
     <t xml:space="preserve">  ☐ Negative test - Delete a non-existing access keys (Google Credentials) @manual</t>
   </si>
   <si>
-    <t>SUITE 49</t>
+    <t>SUITE 50</t>
   </si>
   <si>
     <t xml:space="preserve">4. PreSigned URLs - DCF Staging testing for release sign off - PXP-3836 </t>
   </si>
   <si>
-    <t>SUITE 50</t>
+    <t>SUITE 51</t>
   </si>
   <si>
     <t xml:space="preserve">5. OIDC Flow - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1157,7 +1178,7 @@
     <t xml:space="preserve">  ☐ Perform PreSigned URL test @manual</t>
   </si>
   <si>
-    <t>SUITE 51</t>
+    <t>SUITE 52</t>
   </si>
   <si>
     <t xml:space="preserve">6. IndexD - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1169,13 +1190,13 @@
     <t xml:space="preserve">  ☐ Get controlled data record @manual</t>
   </si>
   <si>
-    <t>SUITE 52</t>
+    <t>SUITE 53</t>
   </si>
   <si>
     <t xml:space="preserve">Export Performance Tests @ExportPerformanceTests @Performance </t>
   </si>
   <si>
-    <t>SUITE 53</t>
+    <t>SUITE 54</t>
   </si>
   <si>
     <t xml:space="preserve">Generate Test Data @GenerateTestData @Performance </t>
@@ -1184,19 +1205,19 @@
     <t xml:space="preserve">  ☐ Generate test data</t>
   </si>
   <si>
-    <t>SUITE 54</t>
+    <t>SUITE 55</t>
   </si>
   <si>
     <t xml:space="preserve">Query Performance Tests @QueryPerformanceTests @Performance </t>
   </si>
   <si>
-    <t>SUITE 55</t>
+    <t>SUITE 56</t>
   </si>
   <si>
     <t xml:space="preserve">Submission Performance Tests @SubmissionPerformanceTests @Performance </t>
   </si>
   <si>
-    <t>SUITE 56</t>
+    <t>SUITE 57</t>
   </si>
   <si>
     <t xml:space="preserve">SubmitAndQueryNodesTest </t>
@@ -1244,7 +1265,7 @@
     <t xml:space="preserve">  ☐ submit data node with consent codes @indexRecordConsentCodes</t>
   </si>
   <si>
-    <t>SUITE 57</t>
+    <t>SUITE 58</t>
   </si>
   <si>
     <t xml:space="preserve">SubmitFileTest </t>
@@ -1259,7 +1280,7 @@
     <t xml:space="preserve">  ☐ submit file then update with URL @reqData</t>
   </si>
   <si>
-    <t>SUITE 58</t>
+    <t>SUITE 59</t>
   </si>
   <si>
     <t xml:space="preserve">Brain Promotion Smoke Test Suite </t>
@@ -1310,7 +1331,7 @@
     <t xml:space="preserve">  ☐ Upload a single file @manual @smoke @brain</t>
   </si>
   <si>
-    <t>SUITE 59</t>
+    <t>SUITE 60</t>
   </si>
   <si>
     <t/>
@@ -1713,7 +1734,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G382"/>
+  <dimension ref="A1:G388"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4845,7 +4866,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="232" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>199</v>
       </c>
@@ -4853,35 +4874,29 @@
         <v>266</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E232" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F232" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="3">
+        <v>200</v>
+      </c>
+      <c r="B233" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="C233" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="3">
-        <v>200</v>
-      </c>
-      <c r="B234" s="3" t="s">
+      <c r="B234" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C234" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>201</v>
       </c>
@@ -4889,26 +4904,29 @@
         <v>270</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="3">
-        <v>202</v>
-      </c>
-      <c r="B236" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F235" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C236" s="3" t="s">
-        <v>10</v>
+      <c r="B236" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="237" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>10</v>
@@ -4916,21 +4934,24 @@
     </row>
     <row r="238" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
+        <v>203</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="3">
         <v>204</v>
       </c>
-      <c r="B238" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B239" s="2" t="s">
+      <c r="B239" s="3" t="s">
         <v>275</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="240" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4955,23 +4976,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="3">
-        <v>207</v>
-      </c>
-      <c r="B242" s="3" t="s">
+    <row r="242" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C242" s="3" t="s">
-        <v>10</v>
+      <c r="B242" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="243" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>10</v>
@@ -4979,10 +4997,10 @@
     </row>
     <row r="244" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A244" s="3">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>10</v>
@@ -4990,24 +5008,27 @@
     </row>
     <row r="245" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
+        <v>209</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="3">
         <v>210</v>
       </c>
-      <c r="B245" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C245" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B246" s="2" t="s">
+      <c r="B246" s="3" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="247" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C246" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>211</v>
       </c>
@@ -5015,16 +5036,10 @@
         <v>284</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E247" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F247" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>212</v>
       </c>
@@ -5032,13 +5047,7 @@
         <v>285</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E248" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F248" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5052,26 +5061,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
+    <row r="250" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="3">
+        <v>214</v>
+      </c>
+      <c r="B250" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B250" s="2" t="s">
+      <c r="C250" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="3">
-        <v>214</v>
-      </c>
-      <c r="B251" s="3" t="s">
+      <c r="B251" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
         <v>215</v>
       </c>
@@ -5079,10 +5088,16 @@
         <v>290</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E252" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F252" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="3">
         <v>216</v>
       </c>
@@ -5090,7 +5105,13 @@
         <v>291</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
+      </c>
+      <c r="E253" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F253" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="254" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5156,34 +5177,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="3">
-        <v>222</v>
-      </c>
-      <c r="B260" s="3" t="s">
+    <row r="260" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C260" s="3" t="s">
-        <v>10</v>
+      <c r="B260" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="261" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" s="3">
+        <v>222</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="3">
         <v>223</v>
       </c>
-      <c r="B261" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="C261" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B262" s="2" t="s">
+      <c r="B262" s="3" t="s">
         <v>302</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="263" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5230,26 +5251,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="267" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="3">
+    <row r="267" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="3">
         <v>228</v>
       </c>
-      <c r="B267" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C267" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B268" s="2" t="s">
+      <c r="B268" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="269" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C268" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="3">
         <v>229</v>
       </c>
@@ -5257,16 +5278,10 @@
         <v>310</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E269" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F269" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="3">
         <v>230</v>
       </c>
@@ -5274,71 +5289,62 @@
         <v>311</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E270" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F270" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="3">
+        <v>231</v>
+      </c>
+      <c r="B271" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B271" s="2" t="s">
+      <c r="C271" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="3">
+        <v>232</v>
+      </c>
+      <c r="B272" s="3" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="272" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="3">
-        <v>231</v>
-      </c>
-      <c r="B272" s="3" t="s">
+      <c r="C272" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C272" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E272" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F272" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A273" s="3">
-        <v>232</v>
-      </c>
-      <c r="B273" s="3" t="s">
+      <c r="B273" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C273" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E273" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F273" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="2" t="s">
+    </row>
+    <row r="274" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="3">
+        <v>233</v>
+      </c>
+      <c r="B274" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="B274" s="2" t="s">
-        <v>317</v>
+      <c r="C274" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E274" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F274" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="275" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="3">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>31</v>
@@ -5352,73 +5358,94 @@
     </row>
     <row r="276" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B276" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B276" s="2" t="s">
+    </row>
+    <row r="277" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="3">
+        <v>235</v>
+      </c>
+      <c r="B277" s="3" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A277" s="3">
-        <v>234</v>
-      </c>
-      <c r="B277" s="3" t="s">
+      <c r="C277" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E277" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F277" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="3">
+        <v>236</v>
+      </c>
+      <c r="B278" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C277" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A278" s="3">
-        <v>235</v>
-      </c>
-      <c r="B278" s="3" t="s">
+      <c r="C278" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E278" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F278" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="3">
+        <v>237</v>
+      </c>
+      <c r="B279" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="C278" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A279" s="3">
-        <v>236</v>
-      </c>
-      <c r="B279" s="3" t="s">
+      <c r="C279" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E279" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F279" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C279" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="3">
-        <v>237</v>
-      </c>
-      <c r="B280" s="3" t="s">
+      <c r="B280" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C280" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A281" s="2" t="s">
+    </row>
+    <row r="281" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="3">
+        <v>238</v>
+      </c>
+      <c r="B281" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B281" s="2" t="s">
+      <c r="C281" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E281" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F281" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A282" s="3">
-        <v>238</v>
-      </c>
-      <c r="B282" s="3" t="s">
+      <c r="B282" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="C282" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="283" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5465,23 +5492,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="3">
-        <v>243</v>
-      </c>
-      <c r="B287" s="3" t="s">
+    <row r="287" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C287" s="3" t="s">
-        <v>10</v>
+      <c r="B287" s="2" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="288" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="3">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>10</v>
@@ -5489,10 +5513,10 @@
     </row>
     <row r="289" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" s="3">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>10</v>
@@ -5500,10 +5524,10 @@
     </row>
     <row r="290" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A290" s="3">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>10</v>
@@ -5511,10 +5535,10 @@
     </row>
     <row r="291" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A291" s="3">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>10</v>
@@ -5522,10 +5546,10 @@
     </row>
     <row r="292" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A292" s="3">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>10</v>
@@ -5533,10 +5557,10 @@
     </row>
     <row r="293" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A293" s="3">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>10</v>
@@ -5544,10 +5568,10 @@
     </row>
     <row r="294" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A294" s="3">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C294" s="3" t="s">
         <v>10</v>
@@ -5555,21 +5579,24 @@
     </row>
     <row r="295" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A295" s="3">
+        <v>250</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C295" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="3">
         <v>251</v>
       </c>
-      <c r="B295" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="C295" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="B296" s="2" t="s">
+      <c r="B296" s="3" t="s">
         <v>342</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="297" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5605,34 +5632,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="2" t="s">
+    <row r="300" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="3">
+        <v>255</v>
+      </c>
+      <c r="B300" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B300" s="2" t="s">
-        <v>347</v>
+      <c r="C300" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="301" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" s="3">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B301" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C301" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C301" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="3">
-        <v>256</v>
-      </c>
-      <c r="B302" s="3" t="s">
+      <c r="B302" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="C302" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="303" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5646,34 +5673,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="2" t="s">
+    <row r="304" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="3">
+        <v>258</v>
+      </c>
+      <c r="B304" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B304" s="2" t="s">
-        <v>352</v>
+      <c r="C304" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="305" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B305" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A306" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C305" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A306" s="3">
-        <v>259</v>
-      </c>
-      <c r="B306" s="3" t="s">
+      <c r="B306" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="C306" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="307" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5703,7 +5730,7 @@
         <v>262</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C309" s="3" t="s">
         <v>10</v>
@@ -5711,10 +5738,10 @@
     </row>
     <row r="310" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="311" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5722,7 +5749,7 @@
         <v>263</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C311" s="3" t="s">
         <v>10</v>
@@ -5733,7 +5760,7 @@
         <v>264</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>10</v>
@@ -5744,7 +5771,7 @@
         <v>265</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>10</v>
@@ -5755,7 +5782,7 @@
         <v>266</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>10</v>
@@ -5766,29 +5793,26 @@
         <v>267</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="3">
-        <v>268</v>
-      </c>
-      <c r="B316" s="3" t="s">
+    <row r="316" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="C316" s="3" t="s">
-        <v>10</v>
+      <c r="B316" s="2" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="317" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>10</v>
@@ -5796,10 +5820,10 @@
     </row>
     <row r="318" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A318" s="3">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>10</v>
@@ -5807,10 +5831,10 @@
     </row>
     <row r="319" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" s="3">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>10</v>
@@ -5818,10 +5842,10 @@
     </row>
     <row r="320" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" s="3">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C320" s="3" t="s">
         <v>10</v>
@@ -5829,10 +5853,10 @@
     </row>
     <row r="321" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" s="3">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>10</v>
@@ -5840,10 +5864,10 @@
     </row>
     <row r="322" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="3">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>10</v>
@@ -5851,21 +5875,24 @@
     </row>
     <row r="323" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3">
+        <v>274</v>
+      </c>
+      <c r="B323" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C323" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="3">
         <v>275</v>
       </c>
-      <c r="B323" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="C323" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A324" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B324" s="2" t="s">
-        <v>370</v>
+      <c r="B324" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C324" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="325" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5873,7 +5900,7 @@
         <v>276</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>10</v>
@@ -5884,7 +5911,7 @@
         <v>277</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>10</v>
@@ -5895,7 +5922,7 @@
         <v>278</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C327" s="3" t="s">
         <v>10</v>
@@ -5906,7 +5933,7 @@
         <v>279</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>10</v>
@@ -5917,7 +5944,7 @@
         <v>280</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>10</v>
@@ -5936,7 +5963,7 @@
         <v>281</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>53</v>
+        <v>378</v>
       </c>
       <c r="C331" s="3" t="s">
         <v>10</v>
@@ -5947,7 +5974,7 @@
         <v>282</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>54</v>
+        <v>379</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>10</v>
@@ -5958,7 +5985,7 @@
         <v>283</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>55</v>
+        <v>380</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>10</v>
@@ -5969,29 +5996,29 @@
         <v>284</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>56</v>
+        <v>381</v>
       </c>
       <c r="C334" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="335" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A335" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B335" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A336" s="3">
+    <row r="335" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="3">
         <v>285</v>
       </c>
-      <c r="B336" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C336" s="3" t="s">
-        <v>10</v>
+      <c r="B335" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C335" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="337" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5999,7 +6026,7 @@
         <v>286</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C337" s="3" t="s">
         <v>10</v>
@@ -6010,207 +6037,168 @@
         <v>287</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>380</v>
+        <v>54</v>
       </c>
       <c r="C338" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="339" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A339" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="B339" s="2" t="s">
-        <v>382</v>
+    <row r="339" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="3">
+        <v>288</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="340" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A340" s="3">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>383</v>
+        <v>56</v>
       </c>
       <c r="C340" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="341" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A341" s="3">
-        <v>289</v>
-      </c>
-      <c r="B341" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="C341" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A342" s="2" t="s">
+    <row r="341" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B342" s="2" t="s">
+      <c r="B341" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="343" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="2" t="s">
+    <row r="342" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="3">
+        <v>290</v>
+      </c>
+      <c r="B342" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C342" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="3">
+        <v>291</v>
+      </c>
+      <c r="B343" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C343" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="3">
+        <v>292</v>
+      </c>
+      <c r="B344" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="B343" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="344" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A344" s="3">
-        <v>290</v>
-      </c>
-      <c r="B344" s="3" t="s">
-        <v>389</v>
-      </c>
       <c r="C344" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E344" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F344" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="345" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="3">
+        <v>293</v>
+      </c>
+      <c r="B346" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="B345" s="2" t="s">
+      <c r="C346" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="3">
+        <v>294</v>
+      </c>
+      <c r="B347" s="3" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="346" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A346" s="2" t="s">
+      <c r="C347" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B346" s="2" t="s">
+      <c r="B348" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="347" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A347" s="2" t="s">
+    <row r="349" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B347" s="2" t="s">
+      <c r="B349" s="2" t="s">
         <v>395</v>
-      </c>
-    </row>
-    <row r="348" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="3">
-        <v>291</v>
-      </c>
-      <c r="B348" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="C348" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E348" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F348" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="349" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="3">
-        <v>292</v>
-      </c>
-      <c r="B349" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C349" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E349" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F349" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="350" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B350" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C350" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E350" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F350" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A351" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B351" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C350" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E350" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F350" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="351" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A351" s="3">
-        <v>294</v>
-      </c>
-      <c r="B351" s="3" t="s">
+    </row>
+    <row r="352" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A352" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C351" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E351" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F351" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="352" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A352" s="3">
-        <v>295</v>
-      </c>
-      <c r="B352" s="3" t="s">
+      <c r="B352" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C352" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E352" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F352" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="353" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A353" s="3">
-        <v>296</v>
-      </c>
-      <c r="B353" s="3" t="s">
+    </row>
+    <row r="353" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C353" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E353" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F353" s="3" t="s">
-        <v>33</v>
+      <c r="B353" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="354" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A354" s="3">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>31</v>
@@ -6224,10 +6212,10 @@
     </row>
     <row r="355" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A355" s="3">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>31</v>
@@ -6241,10 +6229,10 @@
     </row>
     <row r="356" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A356" s="3">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>31</v>
@@ -6258,10 +6246,10 @@
     </row>
     <row r="357" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A357" s="3">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C357" s="3" t="s">
         <v>31</v>
@@ -6275,10 +6263,10 @@
     </row>
     <row r="358" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A358" s="3">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>31</v>
@@ -6292,10 +6280,10 @@
     </row>
     <row r="359" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A359" s="3">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C359" s="3" t="s">
         <v>31</v>
@@ -6309,10 +6297,10 @@
     </row>
     <row r="360" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A360" s="3">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C360" s="3" t="s">
         <v>31</v>
@@ -6326,27 +6314,36 @@
     </row>
     <row r="361" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A361" s="3">
+        <v>303</v>
+      </c>
+      <c r="B361" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C361" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E361" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F361" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="3">
         <v>304</v>
       </c>
-      <c r="B361" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C361" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E361" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F361" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A362" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="B362" s="2" t="s">
+      <c r="B362" s="3" t="s">
         <v>411</v>
+      </c>
+      <c r="C362" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E362" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F362" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="363" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6400,37 +6397,49 @@
         <v>33</v>
       </c>
     </row>
-    <row r="366" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A366" s="2" t="s">
+    <row r="366" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="3">
+        <v>308</v>
+      </c>
+      <c r="B366" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="B366" s="2" t="s">
+      <c r="C366" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E366" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F366" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A367" s="3">
+        <v>309</v>
+      </c>
+      <c r="B367" s="3" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="367" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A367" s="3">
-        <v>308</v>
-      </c>
-      <c r="B367" s="3" t="s">
+      <c r="C367" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E367" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F367" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A368" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C367" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="368" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A368" s="3">
-        <v>309</v>
-      </c>
-      <c r="B368" s="3" t="s">
+      <c r="B368" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="C368" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="369" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="369" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A369" s="3">
         <v>310</v>
       </c>
@@ -6438,10 +6447,16 @@
         <v>419</v>
       </c>
       <c r="C369" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="370" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E369" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F369" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A370" s="3">
         <v>311</v>
       </c>
@@ -6449,10 +6464,16 @@
         <v>420</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="371" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E370" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F370" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A371" s="3">
         <v>312</v>
       </c>
@@ -6460,26 +6481,29 @@
         <v>421</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="372" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A372" s="3">
-        <v>313</v>
-      </c>
-      <c r="B372" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E371" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F371" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A372" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="C372" s="3" t="s">
-        <v>10</v>
+      <c r="B372" s="2" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="373" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A373" s="3">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>10</v>
@@ -6487,10 +6511,10 @@
     </row>
     <row r="374" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A374" s="3">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>10</v>
@@ -6498,10 +6522,10 @@
     </row>
     <row r="375" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>10</v>
@@ -6509,10 +6533,10 @@
     </row>
     <row r="376" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>10</v>
@@ -6520,10 +6544,10 @@
     </row>
     <row r="377" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>10</v>
@@ -6531,10 +6555,10 @@
     </row>
     <row r="378" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>10</v>
@@ -6542,10 +6566,10 @@
     </row>
     <row r="379" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A379" s="3">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>10</v>
@@ -6553,10 +6577,10 @@
     </row>
     <row r="380" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A380" s="3">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>10</v>
@@ -6564,21 +6588,87 @@
     </row>
     <row r="381" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A381" s="3">
+        <v>321</v>
+      </c>
+      <c r="B381" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C381" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="3">
         <v>322</v>
       </c>
-      <c r="B381" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="C381" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="382" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A382" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="B382" s="2" t="s">
+      <c r="B382" s="3" t="s">
         <v>433</v>
+      </c>
+      <c r="C382" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A383" s="3">
+        <v>323</v>
+      </c>
+      <c r="B383" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C383" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A384" s="3">
+        <v>324</v>
+      </c>
+      <c r="B384" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C384" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A385" s="3">
+        <v>325</v>
+      </c>
+      <c r="B385" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C385" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A386" s="3">
+        <v>326</v>
+      </c>
+      <c r="B386" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C386" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A387" s="3">
+        <v>327</v>
+      </c>
+      <c r="B387" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C387" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A388" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -6594,34 +6684,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="C1">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
       <c r="C2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="C3">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C4">
-        <v>322</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
disabling screenshots and updating test plan (#374)
</commit_message>
<xml_diff>
--- a/test-plan.xlsx
+++ b/test-plan.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="444">
   <si>
     <t>S.NO.</t>
   </si>
@@ -809,13 +809,25 @@
     <t>SUITE 32</t>
   </si>
   <si>
+    <t xml:space="preserve">Redirect invalid urls to 404 page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Valid urls are not redirected to 404 page @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Invalid urls get redirected to 404 page @manual</t>
+  </si>
+  <si>
+    <t>SUITE 33</t>
+  </si>
+  <si>
     <t xml:space="preserve">CoreMetadataPageTest </t>
   </si>
   <si>
     <t xml:space="preserve">  ☐ test core metadata page @coreMetadataPage @portal</t>
   </si>
   <si>
-    <t>SUITE 33</t>
+    <t>SUITE 34</t>
   </si>
   <si>
     <t xml:space="preserve">DashboardReports - https://ctds-planx.atlassian.net/browse/PXP-4252 </t>
@@ -836,7 +848,7 @@
     <t xml:space="preserve">  ☐ The dashboard reports gracefully handle no data @manual</t>
   </si>
   <si>
-    <t>SUITE 34</t>
+    <t>SUITE 35</t>
   </si>
   <si>
     <t xml:space="preserve">Data Explorer </t>
@@ -860,7 +872,13 @@
     <t xml:space="preserve">  ☐ Faceted search - Nested data - Nested fields can be shown @manual</t>
   </si>
   <si>
-    <t>SUITE 35</t>
+    <t xml:space="preserve">  ☐ Table - Data displayed in the table is correct @manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ☐ Table - Nested data displayed in the table is correct @manual</t>
+  </si>
+  <si>
+    <t>SUITE 36</t>
   </si>
   <si>
     <t xml:space="preserve">DataUploadTest </t>
@@ -875,7 +893,7 @@
     <t xml:space="preserve">  ☐ Upload clinical data file through portal large enough to trigger chunking @manual @regression</t>
   </si>
   <si>
-    <t>SUITE 36</t>
+    <t>SUITE 37</t>
   </si>
   <si>
     <t xml:space="preserve">ExportToWorkspaceTest </t>
@@ -893,7 +911,7 @@
     <t xml:space="preserve">  ☐ Export default manifest, mount it and check manifest name @exportToWorkspacePortalHatchery @portal @manual</t>
   </si>
   <si>
-    <t>SUITE 37</t>
+    <t>SUITE 38</t>
   </si>
   <si>
     <t xml:space="preserve">File Explorer - https://ctds-planx.atlassian.net/browse/PXP-4777 </t>
@@ -917,7 +935,7 @@
     <t xml:space="preserve">  ☐ Verify labels on the charts in File Explorer page @manual</t>
   </si>
   <si>
-    <t>SUITE 38</t>
+    <t>SUITE 39</t>
   </si>
   <si>
     <t xml:space="preserve">Homepage Chart Nodes </t>
@@ -938,7 +956,7 @@
     <t xml:space="preserve">  ☐ When Homepage Charts is disabled, logged-in users should see summary charts of ONLY the projects they have access to on the landing page @manual</t>
   </si>
   <si>
-    <t>SUITE 39</t>
+    <t>SUITE 40</t>
   </si>
   <si>
     <t xml:space="preserve">Homepage </t>
@@ -950,7 +968,7 @@
     <t xml:space="preserve">  ☐ login @portal @topBarLogin</t>
   </si>
   <si>
-    <t>SUITE 40</t>
+    <t>SUITE 41</t>
   </si>
   <si>
     <t xml:space="preserve">Indexing GUI </t>
@@ -962,7 +980,10 @@
     <t xml:space="preserve">  ☐ Navigate to the indexing page and download a full indexd manifest @indexing</t>
   </si>
   <si>
-    <t>SUITE 41</t>
+    <t xml:space="preserve">  ☐ Navigate to the indexing page and upload an invalid manifest @indexing</t>
+  </si>
+  <si>
+    <t>SUITE 42</t>
   </si>
   <si>
     <t xml:space="preserve">Login </t>
@@ -971,7 +992,7 @@
     <t xml:space="preserve">  ☐ Login redirects to requested page @loginRedirect</t>
   </si>
   <si>
-    <t>SUITE 42</t>
+    <t>SUITE 43</t>
   </si>
   <si>
     <t xml:space="preserve">Windmill configurable profile page </t>
@@ -989,7 +1010,7 @@
     <t xml:space="preserve">  ☐ When configuration has showArboristAuthzOnProfile: false, profile page does not show resources table from Arborist @manual</t>
   </si>
   <si>
-    <t>SUITE 43</t>
+    <t>SUITE 44</t>
   </si>
   <si>
     <t xml:space="preserve">RoleBasedUI - https://ctds-planx.atlassian.net/browse/PXP-4252 </t>
@@ -1037,7 +1058,7 @@
     <t xml:space="preserve">  ☐ The file page download button is not present if the user does not have read-storage permission on the file @manual</t>
   </si>
   <si>
-    <t>SUITE 44</t>
+    <t>SUITE 45</t>
   </si>
   <si>
     <t xml:space="preserve">Terra Export Warning Test Plan </t>
@@ -1052,7 +1073,7 @@
     <t xml:space="preserve">  ☐ When Terra Export Warning is DISABLED, user should NOT be warned when exporting N or more subjects @manual</t>
   </si>
   <si>
-    <t>SUITE 45</t>
+    <t>SUITE 46</t>
   </si>
   <si>
     <t xml:space="preserve">Tiered Access </t>
@@ -1067,7 +1088,7 @@
     <t xml:space="preserve">  ☐ Verify summary charts displayed correctly for partially authorized users @manual @regression @bugfix</t>
   </si>
   <si>
-    <t>SUITE 46</t>
+    <t>SUITE 47</t>
   </si>
   <si>
     <t xml:space="preserve">1. Linking accounts - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1085,7 +1106,7 @@
     <t xml:space="preserve">  ☐ Unlink Google identity from the NIH user @manual</t>
   </si>
   <si>
-    <t>SUITE 47</t>
+    <t>SUITE 48</t>
   </si>
   <si>
     <t xml:space="preserve">2. Service accounts registration - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1121,7 +1142,7 @@
     <t xml:space="preserve">  ☐ Delete existing service account @manual</t>
   </si>
   <si>
-    <t>SUITE 48</t>
+    <t>SUITE 49</t>
   </si>
   <si>
     <t xml:space="preserve">3. Google Credentials - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1142,13 +1163,13 @@
     <t xml:space="preserve">  ☐ Negative test - Delete a non-existing access keys (Google Credentials) @manual</t>
   </si>
   <si>
-    <t>SUITE 49</t>
+    <t>SUITE 50</t>
   </si>
   <si>
     <t xml:space="preserve">4. PreSigned URLs - DCF Staging testing for release sign off - PXP-3836 </t>
   </si>
   <si>
-    <t>SUITE 50</t>
+    <t>SUITE 51</t>
   </si>
   <si>
     <t xml:space="preserve">5. OIDC Flow - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1157,7 +1178,7 @@
     <t xml:space="preserve">  ☐ Perform PreSigned URL test @manual</t>
   </si>
   <si>
-    <t>SUITE 51</t>
+    <t>SUITE 52</t>
   </si>
   <si>
     <t xml:space="preserve">6. IndexD - DCF Staging testing for release sign off - PXP-3836 </t>
@@ -1169,13 +1190,13 @@
     <t xml:space="preserve">  ☐ Get controlled data record @manual</t>
   </si>
   <si>
-    <t>SUITE 52</t>
+    <t>SUITE 53</t>
   </si>
   <si>
     <t xml:space="preserve">Export Performance Tests @ExportPerformanceTests @Performance </t>
   </si>
   <si>
-    <t>SUITE 53</t>
+    <t>SUITE 54</t>
   </si>
   <si>
     <t xml:space="preserve">Generate Test Data @GenerateTestData @Performance </t>
@@ -1184,19 +1205,19 @@
     <t xml:space="preserve">  ☐ Generate test data</t>
   </si>
   <si>
-    <t>SUITE 54</t>
+    <t>SUITE 55</t>
   </si>
   <si>
     <t xml:space="preserve">Query Performance Tests @QueryPerformanceTests @Performance </t>
   </si>
   <si>
-    <t>SUITE 55</t>
+    <t>SUITE 56</t>
   </si>
   <si>
     <t xml:space="preserve">Submission Performance Tests @SubmissionPerformanceTests @Performance </t>
   </si>
   <si>
-    <t>SUITE 56</t>
+    <t>SUITE 57</t>
   </si>
   <si>
     <t xml:space="preserve">SubmitAndQueryNodesTest </t>
@@ -1244,7 +1265,7 @@
     <t xml:space="preserve">  ☐ submit data node with consent codes @indexRecordConsentCodes</t>
   </si>
   <si>
-    <t>SUITE 57</t>
+    <t>SUITE 58</t>
   </si>
   <si>
     <t xml:space="preserve">SubmitFileTest </t>
@@ -1259,7 +1280,7 @@
     <t xml:space="preserve">  ☐ submit file then update with URL @reqData</t>
   </si>
   <si>
-    <t>SUITE 58</t>
+    <t>SUITE 59</t>
   </si>
   <si>
     <t xml:space="preserve">Brain Promotion Smoke Test Suite </t>
@@ -1310,7 +1331,7 @@
     <t xml:space="preserve">  ☐ Upload a single file @manual @smoke @brain</t>
   </si>
   <si>
-    <t>SUITE 59</t>
+    <t>SUITE 60</t>
   </si>
   <si>
     <t/>
@@ -1713,7 +1734,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G382"/>
+  <dimension ref="A1:G388"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4845,7 +4866,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="232" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>199</v>
       </c>
@@ -4853,35 +4874,29 @@
         <v>266</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E232" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F232" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="3">
+        <v>200</v>
+      </c>
+      <c r="B233" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="C233" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="3">
-        <v>200</v>
-      </c>
-      <c r="B234" s="3" t="s">
+      <c r="B234" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C234" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>201</v>
       </c>
@@ -4889,26 +4904,29 @@
         <v>270</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="3">
-        <v>202</v>
-      </c>
-      <c r="B236" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F235" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C236" s="3" t="s">
-        <v>10</v>
+      <c r="B236" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="237" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>10</v>
@@ -4916,21 +4934,24 @@
     </row>
     <row r="238" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
+        <v>203</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="3">
         <v>204</v>
       </c>
-      <c r="B238" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B239" s="2" t="s">
+      <c r="B239" s="3" t="s">
         <v>275</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="240" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4955,23 +4976,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="3">
-        <v>207</v>
-      </c>
-      <c r="B242" s="3" t="s">
+    <row r="242" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C242" s="3" t="s">
-        <v>10</v>
+      <c r="B242" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="243" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>10</v>
@@ -4979,10 +4997,10 @@
     </row>
     <row r="244" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A244" s="3">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>10</v>
@@ -4990,24 +5008,27 @@
     </row>
     <row r="245" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
+        <v>209</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="3">
         <v>210</v>
       </c>
-      <c r="B245" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C245" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B246" s="2" t="s">
+      <c r="B246" s="3" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="247" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C246" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>211</v>
       </c>
@@ -5015,16 +5036,10 @@
         <v>284</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E247" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F247" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>212</v>
       </c>
@@ -5032,13 +5047,7 @@
         <v>285</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E248" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F248" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5052,26 +5061,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
+    <row r="250" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="3">
+        <v>214</v>
+      </c>
+      <c r="B250" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B250" s="2" t="s">
+      <c r="C250" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="3">
-        <v>214</v>
-      </c>
-      <c r="B251" s="3" t="s">
+      <c r="B251" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
         <v>215</v>
       </c>
@@ -5079,10 +5088,16 @@
         <v>290</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E252" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F252" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="3">
         <v>216</v>
       </c>
@@ -5090,7 +5105,13 @@
         <v>291</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
+      </c>
+      <c r="E253" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F253" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="254" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5156,34 +5177,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="3">
-        <v>222</v>
-      </c>
-      <c r="B260" s="3" t="s">
+    <row r="260" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C260" s="3" t="s">
-        <v>10</v>
+      <c r="B260" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="261" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" s="3">
+        <v>222</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="3">
         <v>223</v>
       </c>
-      <c r="B261" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="C261" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B262" s="2" t="s">
+      <c r="B262" s="3" t="s">
         <v>302</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="263" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5230,26 +5251,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="267" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="3">
+    <row r="267" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="3">
         <v>228</v>
       </c>
-      <c r="B267" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C267" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B268" s="2" t="s">
+      <c r="B268" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="269" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C268" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="3">
         <v>229</v>
       </c>
@@ -5257,16 +5278,10 @@
         <v>310</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E269" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F269" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="3">
         <v>230</v>
       </c>
@@ -5274,71 +5289,62 @@
         <v>311</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E270" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F270" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="3">
+        <v>231</v>
+      </c>
+      <c r="B271" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B271" s="2" t="s">
+      <c r="C271" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="3">
+        <v>232</v>
+      </c>
+      <c r="B272" s="3" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="272" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="3">
-        <v>231</v>
-      </c>
-      <c r="B272" s="3" t="s">
+      <c r="C272" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C272" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E272" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F272" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A273" s="3">
-        <v>232</v>
-      </c>
-      <c r="B273" s="3" t="s">
+      <c r="B273" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C273" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E273" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F273" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="2" t="s">
+    </row>
+    <row r="274" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="3">
+        <v>233</v>
+      </c>
+      <c r="B274" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="B274" s="2" t="s">
-        <v>317</v>
+      <c r="C274" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E274" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F274" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="275" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="3">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>31</v>
@@ -5352,73 +5358,94 @@
     </row>
     <row r="276" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B276" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B276" s="2" t="s">
+    </row>
+    <row r="277" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="3">
+        <v>235</v>
+      </c>
+      <c r="B277" s="3" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A277" s="3">
-        <v>234</v>
-      </c>
-      <c r="B277" s="3" t="s">
+      <c r="C277" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E277" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F277" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="3">
+        <v>236</v>
+      </c>
+      <c r="B278" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C277" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A278" s="3">
-        <v>235</v>
-      </c>
-      <c r="B278" s="3" t="s">
+      <c r="C278" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E278" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F278" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="3">
+        <v>237</v>
+      </c>
+      <c r="B279" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="C278" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A279" s="3">
-        <v>236</v>
-      </c>
-      <c r="B279" s="3" t="s">
+      <c r="C279" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E279" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F279" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C279" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="3">
-        <v>237</v>
-      </c>
-      <c r="B280" s="3" t="s">
+      <c r="B280" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C280" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A281" s="2" t="s">
+    </row>
+    <row r="281" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="3">
+        <v>238</v>
+      </c>
+      <c r="B281" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B281" s="2" t="s">
+      <c r="C281" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E281" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F281" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A282" s="3">
-        <v>238</v>
-      </c>
-      <c r="B282" s="3" t="s">
+      <c r="B282" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="C282" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="283" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5465,23 +5492,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="3">
-        <v>243</v>
-      </c>
-      <c r="B287" s="3" t="s">
+    <row r="287" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C287" s="3" t="s">
-        <v>10</v>
+      <c r="B287" s="2" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="288" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A288" s="3">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>10</v>
@@ -5489,10 +5513,10 @@
     </row>
     <row r="289" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" s="3">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>10</v>
@@ -5500,10 +5524,10 @@
     </row>
     <row r="290" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A290" s="3">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>10</v>
@@ -5511,10 +5535,10 @@
     </row>
     <row r="291" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A291" s="3">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>10</v>
@@ -5522,10 +5546,10 @@
     </row>
     <row r="292" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A292" s="3">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>10</v>
@@ -5533,10 +5557,10 @@
     </row>
     <row r="293" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A293" s="3">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>10</v>
@@ -5544,10 +5568,10 @@
     </row>
     <row r="294" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A294" s="3">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C294" s="3" t="s">
         <v>10</v>
@@ -5555,21 +5579,24 @@
     </row>
     <row r="295" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A295" s="3">
+        <v>250</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C295" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="3">
         <v>251</v>
       </c>
-      <c r="B295" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="C295" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="B296" s="2" t="s">
+      <c r="B296" s="3" t="s">
         <v>342</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="297" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5605,34 +5632,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="2" t="s">
+    <row r="300" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="3">
+        <v>255</v>
+      </c>
+      <c r="B300" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B300" s="2" t="s">
-        <v>347</v>
+      <c r="C300" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="301" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A301" s="3">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B301" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C301" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C301" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="3">
-        <v>256</v>
-      </c>
-      <c r="B302" s="3" t="s">
+      <c r="B302" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="C302" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="303" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5646,34 +5673,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="2" t="s">
+    <row r="304" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="3">
+        <v>258</v>
+      </c>
+      <c r="B304" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B304" s="2" t="s">
-        <v>352</v>
+      <c r="C304" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="305" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B305" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A306" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C305" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A306" s="3">
-        <v>259</v>
-      </c>
-      <c r="B306" s="3" t="s">
+      <c r="B306" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="C306" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="307" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5703,7 +5730,7 @@
         <v>262</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C309" s="3" t="s">
         <v>10</v>
@@ -5711,10 +5738,10 @@
     </row>
     <row r="310" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="311" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5722,7 +5749,7 @@
         <v>263</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C311" s="3" t="s">
         <v>10</v>
@@ -5733,7 +5760,7 @@
         <v>264</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C312" s="3" t="s">
         <v>10</v>
@@ -5744,7 +5771,7 @@
         <v>265</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C313" s="3" t="s">
         <v>10</v>
@@ -5755,7 +5782,7 @@
         <v>266</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C314" s="3" t="s">
         <v>10</v>
@@ -5766,29 +5793,26 @@
         <v>267</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C315" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="3">
-        <v>268</v>
-      </c>
-      <c r="B316" s="3" t="s">
+    <row r="316" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="C316" s="3" t="s">
-        <v>10</v>
+      <c r="B316" s="2" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="317" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C317" s="3" t="s">
         <v>10</v>
@@ -5796,10 +5820,10 @@
     </row>
     <row r="318" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A318" s="3">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>10</v>
@@ -5807,10 +5831,10 @@
     </row>
     <row r="319" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" s="3">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C319" s="3" t="s">
         <v>10</v>
@@ -5818,10 +5842,10 @@
     </row>
     <row r="320" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A320" s="3">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C320" s="3" t="s">
         <v>10</v>
@@ -5829,10 +5853,10 @@
     </row>
     <row r="321" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" s="3">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C321" s="3" t="s">
         <v>10</v>
@@ -5840,10 +5864,10 @@
     </row>
     <row r="322" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="3">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C322" s="3" t="s">
         <v>10</v>
@@ -5851,21 +5875,24 @@
     </row>
     <row r="323" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3">
+        <v>274</v>
+      </c>
+      <c r="B323" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C323" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="3">
         <v>275</v>
       </c>
-      <c r="B323" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="C323" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A324" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B324" s="2" t="s">
-        <v>370</v>
+      <c r="B324" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C324" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="325" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5873,7 +5900,7 @@
         <v>276</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C325" s="3" t="s">
         <v>10</v>
@@ -5884,7 +5911,7 @@
         <v>277</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C326" s="3" t="s">
         <v>10</v>
@@ -5895,7 +5922,7 @@
         <v>278</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C327" s="3" t="s">
         <v>10</v>
@@ -5906,7 +5933,7 @@
         <v>279</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C328" s="3" t="s">
         <v>10</v>
@@ -5917,7 +5944,7 @@
         <v>280</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C329" s="3" t="s">
         <v>10</v>
@@ -5936,7 +5963,7 @@
         <v>281</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>53</v>
+        <v>378</v>
       </c>
       <c r="C331" s="3" t="s">
         <v>10</v>
@@ -5947,7 +5974,7 @@
         <v>282</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>54</v>
+        <v>379</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>10</v>
@@ -5958,7 +5985,7 @@
         <v>283</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>55</v>
+        <v>380</v>
       </c>
       <c r="C333" s="3" t="s">
         <v>10</v>
@@ -5969,29 +5996,29 @@
         <v>284</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>56</v>
+        <v>381</v>
       </c>
       <c r="C334" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="335" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A335" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B335" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A336" s="3">
+    <row r="335" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="3">
         <v>285</v>
       </c>
-      <c r="B336" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C336" s="3" t="s">
-        <v>10</v>
+      <c r="B335" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C335" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="337" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5999,7 +6026,7 @@
         <v>286</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C337" s="3" t="s">
         <v>10</v>
@@ -6010,207 +6037,168 @@
         <v>287</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>380</v>
+        <v>54</v>
       </c>
       <c r="C338" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="339" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A339" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="B339" s="2" t="s">
-        <v>382</v>
+    <row r="339" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="3">
+        <v>288</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="340" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A340" s="3">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>383</v>
+        <v>56</v>
       </c>
       <c r="C340" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="341" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A341" s="3">
-        <v>289</v>
-      </c>
-      <c r="B341" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="C341" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A342" s="2" t="s">
+    <row r="341" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B342" s="2" t="s">
+      <c r="B341" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="343" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="2" t="s">
+    <row r="342" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="3">
+        <v>290</v>
+      </c>
+      <c r="B342" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C342" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="3">
+        <v>291</v>
+      </c>
+      <c r="B343" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C343" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="3">
+        <v>292</v>
+      </c>
+      <c r="B344" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="B343" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="344" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A344" s="3">
-        <v>290</v>
-      </c>
-      <c r="B344" s="3" t="s">
-        <v>389</v>
-      </c>
       <c r="C344" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E344" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F344" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="345" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="3">
+        <v>293</v>
+      </c>
+      <c r="B346" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="B345" s="2" t="s">
+      <c r="C346" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="3">
+        <v>294</v>
+      </c>
+      <c r="B347" s="3" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="346" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A346" s="2" t="s">
+      <c r="C347" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B346" s="2" t="s">
+      <c r="B348" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="347" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A347" s="2" t="s">
+    <row r="349" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B347" s="2" t="s">
+      <c r="B349" s="2" t="s">
         <v>395</v>
-      </c>
-    </row>
-    <row r="348" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="3">
-        <v>291</v>
-      </c>
-      <c r="B348" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="C348" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E348" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F348" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="349" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="3">
-        <v>292</v>
-      </c>
-      <c r="B349" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C349" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E349" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F349" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="350" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B350" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C350" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E350" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F350" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A351" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B351" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C350" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E350" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F350" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="351" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A351" s="3">
-        <v>294</v>
-      </c>
-      <c r="B351" s="3" t="s">
+    </row>
+    <row r="352" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A352" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C351" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E351" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F351" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="352" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A352" s="3">
-        <v>295</v>
-      </c>
-      <c r="B352" s="3" t="s">
+      <c r="B352" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C352" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E352" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F352" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="353" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A353" s="3">
-        <v>296</v>
-      </c>
-      <c r="B353" s="3" t="s">
+    </row>
+    <row r="353" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C353" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E353" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F353" s="3" t="s">
-        <v>33</v>
+      <c r="B353" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="354" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A354" s="3">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>31</v>
@@ -6224,10 +6212,10 @@
     </row>
     <row r="355" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A355" s="3">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>31</v>
@@ -6241,10 +6229,10 @@
     </row>
     <row r="356" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A356" s="3">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>31</v>
@@ -6258,10 +6246,10 @@
     </row>
     <row r="357" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A357" s="3">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C357" s="3" t="s">
         <v>31</v>
@@ -6275,10 +6263,10 @@
     </row>
     <row r="358" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A358" s="3">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>31</v>
@@ -6292,10 +6280,10 @@
     </row>
     <row r="359" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A359" s="3">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C359" s="3" t="s">
         <v>31</v>
@@ -6309,10 +6297,10 @@
     </row>
     <row r="360" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A360" s="3">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C360" s="3" t="s">
         <v>31</v>
@@ -6326,27 +6314,36 @@
     </row>
     <row r="361" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A361" s="3">
+        <v>303</v>
+      </c>
+      <c r="B361" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C361" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E361" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F361" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="3">
         <v>304</v>
       </c>
-      <c r="B361" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C361" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E361" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F361" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A362" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="B362" s="2" t="s">
+      <c r="B362" s="3" t="s">
         <v>411</v>
+      </c>
+      <c r="C362" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E362" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F362" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="363" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6400,37 +6397,49 @@
         <v>33</v>
       </c>
     </row>
-    <row r="366" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A366" s="2" t="s">
+    <row r="366" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="3">
+        <v>308</v>
+      </c>
+      <c r="B366" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="B366" s="2" t="s">
+      <c r="C366" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E366" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F366" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A367" s="3">
+        <v>309</v>
+      </c>
+      <c r="B367" s="3" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="367" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A367" s="3">
-        <v>308</v>
-      </c>
-      <c r="B367" s="3" t="s">
+      <c r="C367" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E367" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F367" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A368" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C367" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="368" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A368" s="3">
-        <v>309</v>
-      </c>
-      <c r="B368" s="3" t="s">
+      <c r="B368" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="C368" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="369" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="369" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A369" s="3">
         <v>310</v>
       </c>
@@ -6438,10 +6447,16 @@
         <v>419</v>
       </c>
       <c r="C369" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="370" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E369" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F369" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A370" s="3">
         <v>311</v>
       </c>
@@ -6449,10 +6464,16 @@
         <v>420</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="371" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E370" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F370" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A371" s="3">
         <v>312</v>
       </c>
@@ -6460,26 +6481,29 @@
         <v>421</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="372" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A372" s="3">
-        <v>313</v>
-      </c>
-      <c r="B372" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E371" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F371" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A372" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="C372" s="3" t="s">
-        <v>10</v>
+      <c r="B372" s="2" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="373" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A373" s="3">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>10</v>
@@ -6487,10 +6511,10 @@
     </row>
     <row r="374" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A374" s="3">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>10</v>
@@ -6498,10 +6522,10 @@
     </row>
     <row r="375" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>10</v>
@@ -6509,10 +6533,10 @@
     </row>
     <row r="376" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C376" s="3" t="s">
         <v>10</v>
@@ -6520,10 +6544,10 @@
     </row>
     <row r="377" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>10</v>
@@ -6531,10 +6555,10 @@
     </row>
     <row r="378" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C378" s="3" t="s">
         <v>10</v>
@@ -6542,10 +6566,10 @@
     </row>
     <row r="379" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A379" s="3">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>10</v>
@@ -6553,10 +6577,10 @@
     </row>
     <row r="380" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A380" s="3">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C380" s="3" t="s">
         <v>10</v>
@@ -6564,21 +6588,87 @@
     </row>
     <row r="381" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A381" s="3">
+        <v>321</v>
+      </c>
+      <c r="B381" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C381" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="3">
         <v>322</v>
       </c>
-      <c r="B381" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="C381" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="382" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A382" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="B382" s="2" t="s">
+      <c r="B382" s="3" t="s">
         <v>433</v>
+      </c>
+      <c r="C382" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A383" s="3">
+        <v>323</v>
+      </c>
+      <c r="B383" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C383" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A384" s="3">
+        <v>324</v>
+      </c>
+      <c r="B384" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C384" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A385" s="3">
+        <v>325</v>
+      </c>
+      <c r="B385" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C385" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A386" s="3">
+        <v>326</v>
+      </c>
+      <c r="B386" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C386" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A387" s="3">
+        <v>327</v>
+      </c>
+      <c r="B387" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C387" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A388" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -6594,34 +6684,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="C1">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
       <c r="C2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="C3">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C4">
-        <v>322</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>